<commit_message>
with the correct mean annual precipitation
</commit_message>
<xml_diff>
--- a/with climate data and WWTP coordinate.xlsx
+++ b/with climate data and WWTP coordinate.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bundled!$Z$1:$Z$166</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -959,10 +959,10 @@
     <t>Longtitude</t>
   </si>
   <si>
+    <t>mean annual temperature (celsius degree)</t>
+  </si>
+  <si>
     <t>mean annual precipitation (mm)</t>
-  </si>
-  <si>
-    <t>mean annual temperature (celsius degree)</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1299,8 @@
   <dimension ref="A1:AI166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A1048576"/>
+      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1315,7 @@
     <col min="32" max="32" width="11" style="2"/>
     <col min="33" max="33" width="46.625" style="2" customWidth="1"/>
     <col min="34" max="34" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.75" style="5" customWidth="1"/>
+    <col min="35" max="35" width="30.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -1419,10 +1419,10 @@
         <v>307</v>
       </c>
       <c r="AH1" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AI1" t="s">
         <v>310</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1525,8 +1525,8 @@
       <c r="AH2" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI2" s="5">
-        <v>402.10000737259782</v>
+      <c r="AI2">
+        <v>482.52000884711742</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -1629,8 +1629,8 @@
       <c r="AH3" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI3" s="5">
-        <v>402.10000737259782</v>
+      <c r="AI3">
+        <v>482.52000884711742</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1733,8 +1733,8 @@
       <c r="AH4" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI4" s="5">
-        <v>402.10000737259782</v>
+      <c r="AI4">
+        <v>482.52000884711742</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1837,8 +1837,8 @@
       <c r="AH5" s="5">
         <v>12.141944655051661</v>
       </c>
-      <c r="AI5" s="5">
-        <v>389.35000716211897</v>
+      <c r="AI5">
+        <v>467.22000859454272</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1941,8 +1941,8 @@
       <c r="AH6" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI6" s="5">
-        <v>1053.4027972817421</v>
+      <c r="AI6">
+        <v>1264.0833567380905</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -2045,8 +2045,8 @@
       <c r="AH7" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI7" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI7">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -2149,8 +2149,8 @@
       <c r="AH8" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI8" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI8">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
@@ -2253,8 +2253,8 @@
       <c r="AH9" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI9" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI9">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -2357,8 +2357,8 @@
       <c r="AH10" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI10" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI10">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -2461,8 +2461,8 @@
       <c r="AH11" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI11" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI11">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -2565,8 +2565,8 @@
       <c r="AH12" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI12" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI12">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -2669,8 +2669,8 @@
       <c r="AH13" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI13" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI13">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -2773,8 +2773,8 @@
       <c r="AH14" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI14" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI14">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -2877,8 +2877,8 @@
       <c r="AH15" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI15" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI15">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -2981,8 +2981,8 @@
       <c r="AH16" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI16" s="5">
-        <v>1088.552795794275</v>
+      <c r="AI16">
+        <v>1306.2633549531301</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -3085,8 +3085,8 @@
       <c r="AH17" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI17" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI17">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
@@ -3189,8 +3189,8 @@
       <c r="AH18" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI18" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI18">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -3293,8 +3293,8 @@
       <c r="AH19" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI19" s="5">
-        <v>1088.552795794275</v>
+      <c r="AI19">
+        <v>1306.2633549531301</v>
       </c>
     </row>
     <row r="20" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3397,8 +3397,8 @@
       <c r="AH20" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI20" s="5">
-        <v>1053.4027972817421</v>
+      <c r="AI20">
+        <v>1264.0833567380905</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -3501,8 +3501,8 @@
       <c r="AH21" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI21" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI21">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -3605,8 +3605,8 @@
       <c r="AH22" s="5">
         <v>13.163889099905889</v>
       </c>
-      <c r="AI22" s="5">
-        <v>408.26111831557421</v>
+      <c r="AI22">
+        <v>489.91334197868906</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -3709,8 +3709,8 @@
       <c r="AH23" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI23" s="5">
-        <v>960.15279447370108</v>
+      <c r="AI23">
+        <v>1152.1833533684412</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
@@ -3813,8 +3813,8 @@
       <c r="AH24" s="5">
         <v>17.651111385557385</v>
       </c>
-      <c r="AI24" s="5">
-        <v>955.78890645503998</v>
+      <c r="AI24">
+        <v>1146.9466877460479</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -3917,8 +3917,8 @@
       <c r="AH25" s="5">
         <v>15.193055835366248</v>
       </c>
-      <c r="AI25" s="5">
-        <v>976.17223962810294</v>
+      <c r="AI25">
+        <v>1171.4066875537237</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -4021,8 +4021,8 @@
       <c r="AH26" s="5">
         <v>14.228333567414019</v>
       </c>
-      <c r="AI26" s="5">
-        <v>895.61112764974439</v>
+      <c r="AI26">
+        <v>1074.7333531796933</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -4125,8 +4125,8 @@
       <c r="AH27" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI27" s="5">
-        <v>960.15279447370108</v>
+      <c r="AI27">
+        <v>1152.1833533684412</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -4229,8 +4229,8 @@
       <c r="AH28" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI28" s="5">
-        <v>913.88056923283466</v>
+      <c r="AI28">
+        <v>1096.6566830794015</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -4333,8 +4333,8 @@
       <c r="AH29" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI29" s="5">
-        <v>913.88056923283466</v>
+      <c r="AI29">
+        <v>1096.6566830794015</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -4437,8 +4437,8 @@
       <c r="AH30" s="5">
         <v>15.2763891518116</v>
       </c>
-      <c r="AI30" s="5">
-        <v>911.37779025567909</v>
+      <c r="AI30">
+        <v>1093.6533483068149</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
@@ -4541,8 +4541,8 @@
       <c r="AH31" s="5">
         <v>15.491389160023795</v>
       </c>
-      <c r="AI31" s="5">
-        <v>953.06668441825434</v>
+      <c r="AI31">
+        <v>1143.6800213019053</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -4645,8 +4645,8 @@
       <c r="AH32" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI32" s="5">
-        <v>952.84723995129275</v>
+      <c r="AI32">
+        <v>1143.4166879415511</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
@@ -4749,8 +4749,8 @@
       <c r="AH33" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI33" s="5">
-        <v>952.84723995129275</v>
+      <c r="AI33">
+        <v>1143.4166879415511</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
@@ -4853,8 +4853,8 @@
       <c r="AH34" s="5">
         <v>14.283055821309487</v>
       </c>
-      <c r="AI34" s="5">
-        <v>887.4666805780596</v>
+      <c r="AI34">
+        <v>1064.9600166936716</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
@@ -4957,8 +4957,8 @@
       <c r="AH35" s="5">
         <v>16.284166936079661</v>
       </c>
-      <c r="AI35" s="5">
-        <v>987.07223860422778</v>
+      <c r="AI35">
+        <v>1184.4866863250732</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
@@ -5061,8 +5061,8 @@
       <c r="AH36" s="5">
         <v>18.087500296698675</v>
       </c>
-      <c r="AI36" s="5">
-        <v>938.20279271072809</v>
+      <c r="AI36">
+        <v>1125.8433512528738</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
@@ -5165,8 +5165,8 @@
       <c r="AH37" s="5">
         <v>14.717222467395995</v>
       </c>
-      <c r="AI37" s="5">
-        <v>974.70001626014709</v>
+      <c r="AI37">
+        <v>1169.6400195121764</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
@@ -5272,8 +5272,8 @@
       <c r="AH38" s="5">
         <v>13.463055785890255</v>
       </c>
-      <c r="AI38" s="5">
-        <v>412.66111822426319</v>
+      <c r="AI38">
+        <v>495.19334186911584</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
@@ -5379,8 +5379,8 @@
       <c r="AH39" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI39" s="5">
-        <v>414.8527838024828</v>
+      <c r="AI39">
+        <v>497.82334056297935</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
@@ -5486,8 +5486,8 @@
       <c r="AH40" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI40" s="5">
-        <v>414.8527838024828</v>
+      <c r="AI40">
+        <v>497.82334056297935</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
@@ -5593,8 +5593,8 @@
       <c r="AH41" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI41" s="5">
-        <v>414.8527838024828</v>
+      <c r="AI41">
+        <v>497.82334056297935</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
@@ -5700,8 +5700,8 @@
       <c r="AH42" s="5">
         <v>12.47416684911069</v>
       </c>
-      <c r="AI42" s="5">
-        <v>426.56389491156574</v>
+      <c r="AI42">
+        <v>511.87667389387883</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
@@ -5807,8 +5807,8 @@
       <c r="AH43" s="5">
         <v>10.801666868146922</v>
       </c>
-      <c r="AI43" s="5">
-        <v>425.63334173108967</v>
+      <c r="AI43">
+        <v>510.76001007730764</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
@@ -5914,8 +5914,8 @@
       <c r="AH44" s="5">
         <v>14.008333571544952</v>
       </c>
-      <c r="AI44" s="5">
-        <v>458.97223125956953</v>
+      <c r="AI44">
+        <v>550.76667751148341</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
@@ -6021,8 +6021,8 @@
       <c r="AH45" s="5">
         <v>7.1547223484764499</v>
       </c>
-      <c r="AI45" s="5">
-        <v>324.48611763285265</v>
+      <c r="AI45">
+        <v>389.3833411594232</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.25">
@@ -6128,8 +6128,8 @@
       <c r="AH46" s="5">
         <v>6.6944445381975832</v>
       </c>
-      <c r="AI46" s="5">
-        <v>287.17778201711673</v>
+      <c r="AI46">
+        <v>344.61333842054012</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
@@ -6235,8 +6235,8 @@
       <c r="AH47" s="5">
         <v>4.4341667553409936</v>
       </c>
-      <c r="AI47" s="5">
-        <v>429.1027846506073</v>
+      <c r="AI47">
+        <v>514.92334158072867</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.25">
@@ -6342,8 +6342,8 @@
       <c r="AH48" s="5">
         <v>4.5591666952189476</v>
       </c>
-      <c r="AI48" s="5">
-        <v>352.47222829092709</v>
+      <c r="AI48">
+        <v>422.96667394911248</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.25">
@@ -6449,8 +6449,8 @@
       <c r="AH49" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI49" s="5">
-        <v>585.15834353077742</v>
+      <c r="AI49">
+        <v>702.19001223693294</v>
       </c>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.25">
@@ -6556,8 +6556,8 @@
       <c r="AH50" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI50" s="5">
-        <v>558.05000846460462</v>
+      <c r="AI50">
+        <v>669.66001015752556</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.25">
@@ -6663,8 +6663,8 @@
       <c r="AH51" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI51" s="5">
-        <v>558.05000846460462</v>
+      <c r="AI51">
+        <v>669.66001015752556</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.25">
@@ -6770,8 +6770,8 @@
       <c r="AH52" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI52" s="5">
-        <v>558.05000846460462</v>
+      <c r="AI52">
+        <v>669.66001015752556</v>
       </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
@@ -6877,8 +6877,8 @@
       <c r="AH53" s="5">
         <v>11.009722441848782</v>
       </c>
-      <c r="AI53" s="5">
-        <v>524.06667595584361</v>
+      <c r="AI53">
+        <v>628.88001114701228</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
@@ -6984,8 +6984,8 @@
       <c r="AH54" s="5">
         <v>9.6700001836236975</v>
       </c>
-      <c r="AI54" s="5">
-        <v>552.39167516099076</v>
+      <c r="AI54">
+        <v>662.87001019318893</v>
       </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.25">
@@ -7091,8 +7091,8 @@
       <c r="AH55" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI55" s="5">
-        <v>585.15834353077742</v>
+      <c r="AI55">
+        <v>702.19001223693294</v>
       </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.25">
@@ -7198,8 +7198,8 @@
       <c r="AH56" s="5">
         <v>7.8900001508080297</v>
       </c>
-      <c r="AI56" s="5">
-        <v>538.77223119036194</v>
+      <c r="AI56">
+        <v>646.52667742843425</v>
       </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.25">
@@ -7305,8 +7305,8 @@
       <c r="AH57" s="5">
         <v>5.0902778515799181</v>
       </c>
-      <c r="AI57" s="5">
-        <v>363.45278419926763</v>
+      <c r="AI57">
+        <v>436.14334103912114</v>
       </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
@@ -7412,8 +7412,8 @@
       <c r="AH58" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI58" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI58">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.25">
@@ -7519,8 +7519,8 @@
       <c r="AH59" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI59" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI59">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.25">
@@ -7626,8 +7626,8 @@
       <c r="AH60" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI60" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI60">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.25">
@@ -7733,8 +7733,8 @@
       <c r="AH61" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI61" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI61">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
@@ -7840,8 +7840,8 @@
       <c r="AH62" s="5">
         <v>12.402500250997642</v>
       </c>
-      <c r="AI62" s="5">
-        <v>547.28889729579282</v>
+      <c r="AI62">
+        <v>656.74667675495152</v>
       </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.25">
@@ -7947,8 +7947,8 @@
       <c r="AH63" s="5">
         <v>13.197500290266342</v>
       </c>
-      <c r="AI63" s="5">
-        <v>546.76667534187436</v>
+      <c r="AI63">
+        <v>656.12001041024928</v>
       </c>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.25">
@@ -8054,8 +8054,8 @@
       <c r="AH64" s="5">
         <v>14.578889134505557</v>
       </c>
-      <c r="AI64" s="5">
-        <v>652.91112009332414</v>
+      <c r="AI64">
+        <v>783.4933441119889</v>
       </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.25">
@@ -8161,8 +8161,8 @@
       <c r="AH65" s="5">
         <v>11.883889088572728</v>
       </c>
-      <c r="AI65" s="5">
-        <v>569.71112134224836</v>
+      <c r="AI65">
+        <v>683.65334561069801</v>
       </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.25">
@@ -8268,8 +8268,8 @@
       <c r="AH66" s="5">
         <v>12.213611334106988</v>
       </c>
-      <c r="AI66" s="5">
-        <v>525.42500915875041</v>
+      <c r="AI66">
+        <v>630.5100109905004</v>
       </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.25">
@@ -8375,8 +8375,8 @@
       <c r="AH67" s="5">
         <v>13.395278038394947</v>
       </c>
-      <c r="AI67" s="5">
-        <v>537.2777869978712</v>
+      <c r="AI67">
+        <v>644.73334439744553</v>
       </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.25">
@@ -8482,8 +8482,8 @@
       <c r="AH68" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI68" s="5">
-        <v>566.45556488446891</v>
+      <c r="AI68">
+        <v>679.74667786136274</v>
       </c>
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.25">
@@ -8589,8 +8589,8 @@
       <c r="AH69" s="5">
         <v>14.514166940645211</v>
       </c>
-      <c r="AI69" s="5">
-        <v>596.19445407142246</v>
+      <c r="AI69">
+        <v>715.4333448857069</v>
       </c>
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.25">
@@ -8696,8 +8696,8 @@
       <c r="AH70" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI70" s="5">
-        <v>566.45556488446891</v>
+      <c r="AI70">
+        <v>679.74667786136274</v>
       </c>
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.25">
@@ -8803,8 +8803,8 @@
       <c r="AH71" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI71" s="5">
-        <v>566.45556488446891</v>
+      <c r="AI71">
+        <v>679.74667786136274</v>
       </c>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.25">
@@ -8910,8 +8910,8 @@
       <c r="AH72" s="5">
         <v>13.200278020401795</v>
       </c>
-      <c r="AI72" s="5">
-        <v>570.10278523775446</v>
+      <c r="AI72">
+        <v>684.12334228530528</v>
       </c>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.25">
@@ -9017,8 +9017,8 @@
       <c r="AH73" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI73" s="5">
-        <v>620.17500988518202</v>
+      <c r="AI73">
+        <v>744.21001186221838</v>
       </c>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.25">
@@ -9124,8 +9124,8 @@
       <c r="AH74" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI74" s="5">
-        <v>620.17500988518202</v>
+      <c r="AI74">
+        <v>744.21001186221838</v>
       </c>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.25">
@@ -9231,8 +9231,8 @@
       <c r="AH75" s="5">
         <v>12.714166869243813</v>
       </c>
-      <c r="AI75" s="5">
-        <v>603.38612122357722</v>
+      <c r="AI75">
+        <v>724.0633454682926</v>
       </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.25">
@@ -9338,8 +9338,8 @@
       <c r="AH76" s="5">
         <v>14.380278021987113</v>
       </c>
-      <c r="AI76" s="5">
-        <v>491.92778695105682</v>
+      <c r="AI76">
+        <v>590.31334434126813</v>
       </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.25">
@@ -9445,8 +9445,8 @@
       <c r="AH77" s="5">
         <v>15.016111336586375</v>
       </c>
-      <c r="AI77" s="5">
-        <v>523.51389659030576</v>
+      <c r="AI77">
+        <v>628.21667590836682</v>
       </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.25">
@@ -9552,8 +9552,8 @@
       <c r="AH78" s="5">
         <v>14.131666897899574</v>
       </c>
-      <c r="AI78" s="5">
-        <v>609.11667874124316</v>
+      <c r="AI78">
+        <v>730.94001448949177</v>
       </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.25">
@@ -9659,8 +9659,8 @@
       <c r="AH79" s="5">
         <v>14.880833575605518</v>
       </c>
-      <c r="AI79" s="5">
-        <v>559.15000913561221</v>
+      <c r="AI79">
+        <v>670.98001096273458</v>
       </c>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.25">
@@ -9766,8 +9766,8 @@
       <c r="AH80" s="5">
         <v>16.243055798009866</v>
       </c>
-      <c r="AI80" s="5">
-        <v>974.54724013743305</v>
+      <c r="AI80">
+        <v>1169.4566881649196</v>
       </c>
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.25">
@@ -9873,8 +9873,8 @@
       <c r="AH81" s="5">
         <v>16.389166925619875</v>
       </c>
-      <c r="AI81" s="5">
-        <v>1045.9916839278819</v>
+      <c r="AI81">
+        <v>1255.1900207134584</v>
       </c>
     </row>
     <row r="82" spans="1:35" x14ac:dyDescent="0.25">
@@ -9980,8 +9980,8 @@
       <c r="AH82" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI82" s="5">
-        <v>972.81945985162429</v>
+      <c r="AI82">
+        <v>1167.3833518219492</v>
       </c>
     </row>
     <row r="83" spans="1:35" x14ac:dyDescent="0.25">
@@ -10087,8 +10087,8 @@
       <c r="AH83" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI83" s="5">
-        <v>972.81945985162429</v>
+      <c r="AI83">
+        <v>1167.3833518219492</v>
       </c>
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.25">
@@ -10194,8 +10194,8 @@
       <c r="AH84" s="5">
         <v>15.054166897386313</v>
       </c>
-      <c r="AI84" s="5">
-        <v>680.59445726954277</v>
+      <c r="AI84">
+        <v>816.7133487234513</v>
       </c>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.25">
@@ -10301,8 +10301,8 @@
       <c r="AH85" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI85" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI85">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.25">
@@ -10408,8 +10408,8 @@
       <c r="AH86" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI86" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI86">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.25">
@@ -10515,8 +10515,8 @@
       <c r="AH87" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI87" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI87">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.25">
@@ -10622,8 +10622,8 @@
       <c r="AH88" s="5">
         <v>16.396111346284549</v>
       </c>
-      <c r="AI88" s="5">
-        <v>1023.2333520479086</v>
+      <c r="AI88">
+        <v>1227.8800224574904</v>
       </c>
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.25">
@@ -10729,8 +10729,8 @@
       <c r="AH89" s="5">
         <v>15.944722454353339</v>
       </c>
-      <c r="AI89" s="5">
-        <v>973.28057178854942</v>
+      <c r="AI89">
+        <v>1167.9366861462593</v>
       </c>
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.25">
@@ -10836,8 +10836,8 @@
       <c r="AH90" s="5">
         <v>15.40638912299441</v>
       </c>
-      <c r="AI90" s="5">
-        <v>937.34723641309472</v>
+      <c r="AI90">
+        <v>1124.8166836957137</v>
       </c>
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.25">
@@ -10943,8 +10943,8 @@
       <c r="AH91" s="5">
         <v>14.980833584670391</v>
       </c>
-      <c r="AI91" s="5">
-        <v>755.10834456897442</v>
+      <c r="AI91">
+        <v>906.1300134827693</v>
       </c>
     </row>
     <row r="92" spans="1:35" x14ac:dyDescent="0.25">
@@ -11050,8 +11050,8 @@
       <c r="AH92" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI92" s="5">
-        <v>916.66668113569415</v>
+      <c r="AI92">
+        <v>1100.000017362833</v>
       </c>
     </row>
     <row r="93" spans="1:35" x14ac:dyDescent="0.25">
@@ -11157,8 +11157,8 @@
       <c r="AH93" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI93" s="5">
-        <v>916.66668113569415</v>
+      <c r="AI93">
+        <v>1100.000017362833</v>
       </c>
     </row>
     <row r="94" spans="1:35" x14ac:dyDescent="0.25">
@@ -11264,8 +11264,8 @@
       <c r="AH94" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI94" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI94">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.25">
@@ -11371,8 +11371,8 @@
       <c r="AH95" s="5">
         <v>15.691944675313103</v>
       </c>
-      <c r="AI95" s="5">
-        <v>918.32779509491388</v>
+      <c r="AI95">
+        <v>1101.9933541138967</v>
       </c>
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.25">
@@ -11478,8 +11478,8 @@
       <c r="AH96" s="5">
         <v>15.582500197138224</v>
       </c>
-      <c r="AI96" s="5">
-        <v>711.19723644293845</v>
+      <c r="AI96">
+        <v>853.43668373152616</v>
       </c>
     </row>
     <row r="97" spans="1:35" x14ac:dyDescent="0.25">
@@ -11585,8 +11585,8 @@
       <c r="AH97" s="5">
         <v>16.058055824786425</v>
       </c>
-      <c r="AI97" s="5">
-        <v>808.70001078314249</v>
+      <c r="AI97">
+        <v>970.44001293977101</v>
       </c>
     </row>
     <row r="98" spans="1:35" x14ac:dyDescent="0.25">
@@ -11692,8 +11692,8 @@
       <c r="AH98" s="5">
         <v>15.946111321780418</v>
       </c>
-      <c r="AI98" s="5">
-        <v>830.38057103566825</v>
+      <c r="AI98">
+        <v>996.45668524280188</v>
       </c>
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.25">
@@ -11799,8 +11799,8 @@
       <c r="AH99" s="5">
         <v>16.454722446203231</v>
       </c>
-      <c r="AI99" s="5">
-        <v>965.53890664647849</v>
+      <c r="AI99">
+        <v>1158.6466879757743</v>
       </c>
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.25">
@@ -11906,8 +11906,8 @@
       <c r="AH100" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI100" s="5">
-        <v>1177.1250198669732</v>
+      <c r="AI100">
+        <v>1412.5500238403679</v>
       </c>
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.25">
@@ -12013,8 +12013,8 @@
       <c r="AH101" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI101" s="5">
-        <v>1177.1250198669732</v>
+      <c r="AI101">
+        <v>1412.5500238403679</v>
       </c>
     </row>
     <row r="102" spans="1:35" x14ac:dyDescent="0.25">
@@ -12120,8 +12120,8 @@
       <c r="AH102" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI102" s="5">
-        <v>1177.1250198669732</v>
+      <c r="AI102">
+        <v>1412.5500238403679</v>
       </c>
     </row>
     <row r="103" spans="1:35" x14ac:dyDescent="0.25">
@@ -12227,8 +12227,8 @@
       <c r="AH103" s="5">
         <v>15.962500282625358</v>
       </c>
-      <c r="AI103" s="5">
-        <v>1251.4500212321677</v>
+      <c r="AI103">
+        <v>1501.7400254786014</v>
       </c>
     </row>
     <row r="104" spans="1:35" x14ac:dyDescent="0.25">
@@ -12334,8 +12334,8 @@
       <c r="AH104" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI104" s="5">
-        <v>1191.1305749962728</v>
+      <c r="AI104">
+        <v>1429.3566899955272</v>
       </c>
     </row>
     <row r="105" spans="1:35" x14ac:dyDescent="0.25">
@@ -12441,8 +12441,8 @@
       <c r="AH105" s="5">
         <v>17.36972248951594</v>
       </c>
-      <c r="AI105" s="5">
-        <v>1349.7722442580593</v>
+      <c r="AI105">
+        <v>1619.7266931096713</v>
       </c>
     </row>
     <row r="106" spans="1:35" x14ac:dyDescent="0.25">
@@ -12548,8 +12548,8 @@
       <c r="AH106" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI106" s="5">
-        <v>1191.1305749962728</v>
+      <c r="AI106">
+        <v>1429.3566899955272</v>
       </c>
     </row>
     <row r="107" spans="1:35" x14ac:dyDescent="0.25">
@@ -12655,8 +12655,8 @@
       <c r="AH107" s="5">
         <v>16.991666977935367</v>
       </c>
-      <c r="AI107" s="5">
-        <v>1217.8805788490508</v>
+      <c r="AI107">
+        <v>1461.4566946188609</v>
       </c>
     </row>
     <row r="108" spans="1:35" x14ac:dyDescent="0.25">
@@ -12762,8 +12762,8 @@
       <c r="AH108" s="5">
         <v>17.177500254909198</v>
       </c>
-      <c r="AI108" s="5">
-        <v>1147.3750202815152</v>
+      <c r="AI108">
+        <v>1376.8500243378182</v>
       </c>
     </row>
     <row r="109" spans="1:35" x14ac:dyDescent="0.25">
@@ -12869,8 +12869,8 @@
       <c r="AH109" s="5">
         <v>16.59805584020085</v>
       </c>
-      <c r="AI109" s="5">
-        <v>1339.4305793709225</v>
+      <c r="AI109">
+        <v>1607.316695245107</v>
       </c>
     </row>
     <row r="110" spans="1:35" x14ac:dyDescent="0.25">
@@ -12976,8 +12976,8 @@
       <c r="AH110" s="5">
         <v>18.400555811987982</v>
       </c>
-      <c r="AI110" s="5">
-        <v>1391.8944691154693</v>
+      <c r="AI110">
+        <v>1670.273362938563</v>
       </c>
     </row>
     <row r="111" spans="1:35" x14ac:dyDescent="0.25">
@@ -13083,8 +13083,8 @@
       <c r="AH111" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI111" s="5">
-        <v>1104.4277913001263</v>
+      <c r="AI111">
+        <v>1325.3133495601514</v>
       </c>
     </row>
     <row r="112" spans="1:35" x14ac:dyDescent="0.25">
@@ -13190,8 +13190,8 @@
       <c r="AH112" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI112" s="5">
-        <v>1104.4277913001263</v>
+      <c r="AI112">
+        <v>1325.3133495601514</v>
       </c>
     </row>
     <row r="113" spans="1:35" x14ac:dyDescent="0.25">
@@ -13297,8 +13297,8 @@
       <c r="AH113" s="5">
         <v>16.237500274015797</v>
       </c>
-      <c r="AI113" s="5">
-        <v>1115.8777972248693</v>
+      <c r="AI113">
+        <v>1339.0533566698432</v>
       </c>
     </row>
     <row r="114" spans="1:35" x14ac:dyDescent="0.25">
@@ -13404,8 +13404,8 @@
       <c r="AH114" s="5">
         <v>16.611111394564311</v>
       </c>
-      <c r="AI114" s="5">
-        <v>1209.9305740810103</v>
+      <c r="AI114">
+        <v>1451.9166888972125</v>
       </c>
     </row>
     <row r="115" spans="1:35" x14ac:dyDescent="0.25">
@@ -13511,8 +13511,8 @@
       <c r="AH115" s="5">
         <v>16.962222494681676</v>
       </c>
-      <c r="AI115" s="5">
-        <v>1292.7444617682033</v>
+      <c r="AI115">
+        <v>1551.293354121844</v>
       </c>
     </row>
     <row r="116" spans="1:35" x14ac:dyDescent="0.25">
@@ -13618,8 +13618,8 @@
       <c r="AH116" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI116" s="5">
-        <v>1253.5278008513981</v>
+      <c r="AI116">
+        <v>1504.2333610216776</v>
       </c>
     </row>
     <row r="117" spans="1:35" x14ac:dyDescent="0.25">
@@ -13725,8 +13725,8 @@
       <c r="AH117" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI117" s="5">
-        <v>1253.5278008513981</v>
+      <c r="AI117">
+        <v>1504.2333610216776</v>
       </c>
     </row>
     <row r="118" spans="1:35" x14ac:dyDescent="0.25">
@@ -13832,8 +13832,8 @@
       <c r="AH118" s="5">
         <v>17.300555813312531</v>
       </c>
-      <c r="AI118" s="5">
-        <v>1423.0694724387592</v>
+      <c r="AI118">
+        <v>1707.6833669265111</v>
       </c>
     </row>
     <row r="119" spans="1:35" x14ac:dyDescent="0.25">
@@ -13939,8 +13939,8 @@
       <c r="AH119" s="5">
         <v>16.892500269412995</v>
       </c>
-      <c r="AI119" s="5">
-        <v>1336.4194651179844</v>
+      <c r="AI119">
+        <v>1603.7033581415812</v>
       </c>
     </row>
     <row r="120" spans="1:35" x14ac:dyDescent="0.25">
@@ -14046,8 +14046,8 @@
       <c r="AH120" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI120" s="5">
-        <v>1283.6750270724297</v>
+      <c r="AI120">
+        <v>1540.4100324869155</v>
       </c>
     </row>
     <row r="121" spans="1:35" x14ac:dyDescent="0.25">
@@ -14153,8 +14153,8 @@
       <c r="AH121" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI121" s="5">
-        <v>1283.6750270724297</v>
+      <c r="AI121">
+        <v>1540.4100324869155</v>
       </c>
     </row>
     <row r="122" spans="1:35" x14ac:dyDescent="0.25">
@@ -14260,8 +14260,8 @@
       <c r="AH122" s="5">
         <v>17.377222496933406</v>
       </c>
-      <c r="AI122" s="5">
-        <v>1343.3778014977772</v>
+      <c r="AI122">
+        <v>1612.0533617973329</v>
       </c>
     </row>
     <row r="123" spans="1:35" x14ac:dyDescent="0.25">
@@ -14367,8 +14367,8 @@
       <c r="AH123" s="5">
         <v>18.61972255706787</v>
       </c>
-      <c r="AI123" s="5">
-        <v>1319.411135070854</v>
+      <c r="AI123">
+        <v>1583.2933620850245</v>
       </c>
     </row>
     <row r="124" spans="1:35" x14ac:dyDescent="0.25">
@@ -14474,8 +14474,8 @@
       <c r="AH124" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI124" s="5">
-        <v>1485.5694680930012</v>
+      <c r="AI124">
+        <v>1782.6833617116015</v>
       </c>
     </row>
     <row r="125" spans="1:35" x14ac:dyDescent="0.25">
@@ -14581,8 +14581,8 @@
       <c r="AH125" s="5">
         <v>21.330278105205959</v>
       </c>
-      <c r="AI125" s="5">
-        <v>1181.3278022805848</v>
+      <c r="AI125">
+        <v>1417.5933627367019</v>
       </c>
     </row>
     <row r="126" spans="1:35" x14ac:dyDescent="0.25">
@@ -14688,8 +14688,8 @@
       <c r="AH126" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI126" s="5">
-        <v>1485.5694680930012</v>
+      <c r="AI126">
+        <v>1782.6833617116015</v>
       </c>
     </row>
     <row r="127" spans="1:35" x14ac:dyDescent="0.25">
@@ -14795,8 +14795,8 @@
       <c r="AH127" s="5">
         <v>14.705277992950545</v>
       </c>
-      <c r="AI127" s="5">
-        <v>545.45556631498039</v>
+      <c r="AI127">
+        <v>654.54667957797642</v>
       </c>
     </row>
     <row r="128" spans="1:35" x14ac:dyDescent="0.25">
@@ -14902,8 +14902,8 @@
       <c r="AH128" s="5">
         <v>15.146666885043183</v>
       </c>
-      <c r="AI128" s="5">
-        <v>511.14445323290101</v>
+      <c r="AI128">
+        <v>613.37334387948113</v>
       </c>
     </row>
     <row r="129" spans="1:35" x14ac:dyDescent="0.25">
@@ -15009,8 +15009,8 @@
       <c r="AH129" s="5">
         <v>15.114166894327436</v>
       </c>
-      <c r="AI129" s="5">
-        <v>552.70001020903385</v>
+      <c r="AI129">
+        <v>663.24001225084066</v>
       </c>
     </row>
     <row r="130" spans="1:35" x14ac:dyDescent="0.25">
@@ -15116,8 +15116,8 @@
       <c r="AH130" s="5">
         <v>14.685000222010745</v>
       </c>
-      <c r="AI130" s="5">
-        <v>516.12222921537852</v>
+      <c r="AI130">
+        <v>619.34667505845425</v>
       </c>
     </row>
     <row r="131" spans="1:35" x14ac:dyDescent="0.25">
@@ -15223,8 +15223,8 @@
       <c r="AH131" s="5">
         <v>14.560555819484096</v>
       </c>
-      <c r="AI131" s="5">
-        <v>486.50834265165031</v>
+      <c r="AI131">
+        <v>583.81001118198037</v>
       </c>
     </row>
     <row r="132" spans="1:35" x14ac:dyDescent="0.25">
@@ -15330,8 +15330,8 @@
       <c r="AH132" s="5">
         <v>14.925000269276401</v>
       </c>
-      <c r="AI132" s="5">
-        <v>587.93612111028699</v>
+      <c r="AI132">
+        <v>705.52334533234432</v>
       </c>
     </row>
     <row r="133" spans="1:35" x14ac:dyDescent="0.25">
@@ -15437,8 +15437,8 @@
       <c r="AH133" s="5">
         <v>14.240833549056616</v>
       </c>
-      <c r="AI133" s="5">
-        <v>578.55278752330275</v>
+      <c r="AI133">
+        <v>694.26334502796328</v>
       </c>
     </row>
     <row r="134" spans="1:35" x14ac:dyDescent="0.25">
@@ -15544,8 +15544,8 @@
       <c r="AH134" s="5">
         <v>15.481111367895371</v>
       </c>
-      <c r="AI134" s="5">
-        <v>664.15001225223148</v>
+      <c r="AI134">
+        <v>796.98001470267775</v>
       </c>
     </row>
     <row r="135" spans="1:35" x14ac:dyDescent="0.25">
@@ -15651,8 +15651,8 @@
       <c r="AH135" s="5">
         <v>15.808611411021815</v>
       </c>
-      <c r="AI135" s="5">
-        <v>732.42223528027534</v>
+      <c r="AI135">
+        <v>878.90668233633039</v>
       </c>
     </row>
     <row r="136" spans="1:35" x14ac:dyDescent="0.25">
@@ -15758,8 +15758,8 @@
       <c r="AH136" s="5">
         <v>16.348055789868038</v>
       </c>
-      <c r="AI136" s="5">
-        <v>706.5083447649248</v>
+      <c r="AI136">
+        <v>847.81001371790967</v>
       </c>
     </row>
     <row r="137" spans="1:35" x14ac:dyDescent="0.25">
@@ -15865,8 +15865,8 @@
       <c r="AH137" s="5">
         <v>13.885278014466166</v>
       </c>
-      <c r="AI137" s="5">
-        <v>482.41945241867666</v>
+      <c r="AI137">
+        <v>578.90334290241196</v>
       </c>
     </row>
     <row r="138" spans="1:35" x14ac:dyDescent="0.25">
@@ -15972,8 +15972,8 @@
       <c r="AH138" s="5">
         <v>17.218055825101004</v>
       </c>
-      <c r="AI138" s="5">
-        <v>1039.4416841963928</v>
+      <c r="AI138">
+        <v>1247.3300210356713</v>
       </c>
     </row>
     <row r="139" spans="1:35" x14ac:dyDescent="0.25">
@@ -16079,8 +16079,8 @@
       <c r="AH139" s="5">
         <v>17.671944708956612</v>
       </c>
-      <c r="AI139" s="5">
-        <v>1200.402797886067</v>
+      <c r="AI139">
+        <v>1440.4833574632803</v>
       </c>
     </row>
     <row r="140" spans="1:35" x14ac:dyDescent="0.25">
@@ -16186,8 +16186,8 @@
       <c r="AH140" s="5">
         <v>17.840000283055836</v>
       </c>
-      <c r="AI140" s="5">
-        <v>1233.1194645899038</v>
+      <c r="AI140">
+        <v>1479.7433575078844</v>
       </c>
     </row>
     <row r="141" spans="1:35" x14ac:dyDescent="0.25">
@@ -16293,8 +16293,8 @@
       <c r="AH141" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI141" s="5">
-        <v>1830.8222555894818</v>
+      <c r="AI141">
+        <v>2196.9867067073783</v>
       </c>
     </row>
     <row r="142" spans="1:35" x14ac:dyDescent="0.25">
@@ -16400,8 +16400,8 @@
       <c r="AH142" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI142" s="5">
-        <v>1830.8222555894818</v>
+      <c r="AI142">
+        <v>2196.9867067073783</v>
       </c>
     </row>
     <row r="143" spans="1:35" x14ac:dyDescent="0.25">
@@ -16507,8 +16507,8 @@
       <c r="AH143" s="5">
         <v>22.497500356038412</v>
       </c>
-      <c r="AI143" s="5">
-        <v>1457.10002325558</v>
+      <c r="AI143">
+        <v>1748.520027906696</v>
       </c>
     </row>
     <row r="144" spans="1:35" x14ac:dyDescent="0.25">
@@ -16614,8 +16614,8 @@
       <c r="AH144" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI144" s="5">
-        <v>834.33056925133701</v>
+      <c r="AI144">
+        <v>1001.1966831016044</v>
       </c>
     </row>
     <row r="145" spans="1:35" x14ac:dyDescent="0.25">
@@ -16721,8 +16721,8 @@
       <c r="AH145" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI145" s="5">
-        <v>834.33056925133701</v>
+      <c r="AI145">
+        <v>1001.1966831016044</v>
       </c>
     </row>
     <row r="146" spans="1:35" x14ac:dyDescent="0.25">
@@ -16828,8 +16828,8 @@
       <c r="AH146" s="5">
         <v>16.466389189826117</v>
       </c>
-      <c r="AI146" s="5">
-        <v>841.05279137276943</v>
+      <c r="AI146">
+        <v>1009.2633496473233</v>
       </c>
     </row>
     <row r="147" spans="1:35" x14ac:dyDescent="0.25">
@@ -16935,8 +16935,8 @@
       <c r="AH147" s="5">
         <v>18.550555888811747</v>
       </c>
-      <c r="AI147" s="5">
-        <v>921.3805729982754</v>
+      <c r="AI147">
+        <v>1105.6566875979304</v>
       </c>
     </row>
     <row r="148" spans="1:35" x14ac:dyDescent="0.25">
@@ -17042,8 +17042,8 @@
       <c r="AH148" s="5">
         <v>16.811666933695474</v>
       </c>
-      <c r="AI148" s="5">
-        <v>773.31945808397393</v>
+      <c r="AI148">
+        <v>927.98334970076883</v>
       </c>
     </row>
     <row r="149" spans="1:35" x14ac:dyDescent="0.25">
@@ -17149,8 +17149,8 @@
       <c r="AH149" s="5">
         <v>16.939166976345909</v>
       </c>
-      <c r="AI149" s="5">
-        <v>819.41945890420016</v>
+      <c r="AI149">
+        <v>983.30335068504019</v>
       </c>
     </row>
     <row r="150" spans="1:35" x14ac:dyDescent="0.25">
@@ -17256,8 +17256,8 @@
       <c r="AH150" s="5">
         <v>17.050555853048959</v>
       </c>
-      <c r="AI150" s="5">
-        <v>892.72501441505233</v>
+      <c r="AI150">
+        <v>1071.2700172980626</v>
       </c>
     </row>
     <row r="151" spans="1:35" x14ac:dyDescent="0.25">
@@ -17363,8 +17363,8 @@
       <c r="AH151" s="5">
         <v>18.485833643542396</v>
       </c>
-      <c r="AI151" s="5">
-        <v>872.06945833232669</v>
+      <c r="AI151">
+        <v>1046.4833499987919</v>
       </c>
     </row>
     <row r="152" spans="1:35" x14ac:dyDescent="0.25">
@@ -17470,8 +17470,8 @@
       <c r="AH152" s="5">
         <v>17.482500301467049</v>
       </c>
-      <c r="AI152" s="5">
-        <v>860.67501521627935</v>
+      <c r="AI152">
+        <v>1032.8100182595351</v>
       </c>
     </row>
     <row r="153" spans="1:35" x14ac:dyDescent="0.25">
@@ -17577,8 +17577,8 @@
       <c r="AH153" s="5">
         <v>17.544166929192013</v>
       </c>
-      <c r="AI153" s="5">
-        <v>887.32223747173953</v>
+      <c r="AI153">
+        <v>1064.7866849660873</v>
       </c>
     </row>
     <row r="154" spans="1:35" x14ac:dyDescent="0.25">
@@ -17684,8 +17684,8 @@
       <c r="AH154" s="5">
         <v>17.002222526735729</v>
       </c>
-      <c r="AI154" s="5">
-        <v>907.56946346494885</v>
+      <c r="AI154">
+        <v>1089.0833561579386</v>
       </c>
     </row>
     <row r="155" spans="1:35" x14ac:dyDescent="0.25">
@@ -17791,8 +17791,8 @@
       <c r="AH155" s="5">
         <v>16.162500272856818</v>
       </c>
-      <c r="AI155" s="5">
-        <v>937.16668129629556</v>
+      <c r="AI155">
+        <v>1124.6000175555548</v>
       </c>
     </row>
     <row r="156" spans="1:35" x14ac:dyDescent="0.25">
@@ -17898,8 +17898,8 @@
       <c r="AH156" s="5">
         <v>13.510278080569373</v>
       </c>
-      <c r="AI156" s="5">
-        <v>787.63334739849802</v>
+      <c r="AI156">
+        <v>945.16001687819755</v>
       </c>
     </row>
     <row r="157" spans="1:35" x14ac:dyDescent="0.25">
@@ -18005,8 +18005,8 @@
       <c r="AH157" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI157" s="5">
-        <v>549.71389919084811</v>
+      <c r="AI157">
+        <v>659.65667902901771</v>
       </c>
     </row>
     <row r="158" spans="1:35" x14ac:dyDescent="0.25">
@@ -18112,8 +18112,8 @@
       <c r="AH158" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI158" s="5">
-        <v>549.71389919084811</v>
+      <c r="AI158">
+        <v>659.65667902901771</v>
       </c>
     </row>
     <row r="159" spans="1:35" x14ac:dyDescent="0.25">
@@ -18219,8 +18219,8 @@
       <c r="AH159" s="5">
         <v>11.430000214464963</v>
       </c>
-      <c r="AI159" s="5">
-        <v>464.2444530808263</v>
+      <c r="AI159">
+        <v>557.09334369699161</v>
       </c>
     </row>
     <row r="160" spans="1:35" x14ac:dyDescent="0.25">
@@ -18326,8 +18326,8 @@
       <c r="AH160" s="5">
         <v>7.7977779119999875</v>
       </c>
-      <c r="AI160" s="5">
-        <v>304.89444963427053</v>
+      <c r="AI160">
+        <v>365.87333956112462</v>
       </c>
     </row>
     <row r="161" spans="1:35" x14ac:dyDescent="0.25">
@@ -18433,8 +18433,8 @@
       <c r="AH161" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI161" s="5">
-        <v>186.40278092482023</v>
+      <c r="AI161">
+        <v>223.68333710978428</v>
       </c>
     </row>
     <row r="162" spans="1:35" x14ac:dyDescent="0.25">
@@ -18540,8 +18540,8 @@
       <c r="AH162" s="5">
         <v>7.6125001351452539</v>
       </c>
-      <c r="AI162" s="5">
-        <v>318.32222728969322</v>
+      <c r="AI162">
+        <v>381.98667274763187</v>
       </c>
     </row>
     <row r="163" spans="1:35" x14ac:dyDescent="0.25">
@@ -18647,8 +18647,8 @@
       <c r="AH163" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI163" s="5">
-        <v>186.40278092482023</v>
+      <c r="AI163">
+        <v>223.68333710978428</v>
       </c>
     </row>
     <row r="164" spans="1:35" x14ac:dyDescent="0.25">
@@ -18754,8 +18754,8 @@
       <c r="AH164" s="5">
         <v>5.8491667841457655</v>
       </c>
-      <c r="AI164" s="5">
-        <v>183.68611463511155</v>
+      <c r="AI164">
+        <v>220.42333756213387</v>
       </c>
     </row>
     <row r="165" spans="1:35" x14ac:dyDescent="0.25">
@@ -18861,8 +18861,8 @@
       <c r="AH165" s="5">
         <v>4.4586112032747929</v>
       </c>
-      <c r="AI165" s="5">
-        <v>193.72222591543363</v>
+      <c r="AI165">
+        <v>232.46667109852035</v>
       </c>
     </row>
     <row r="166" spans="1:35" x14ac:dyDescent="0.25">
@@ -18968,8 +18968,8 @@
       <c r="AH166" s="5">
         <v>5.5380556673639347</v>
       </c>
-      <c r="AI166" s="5">
-        <v>173.45555842088328</v>
+      <c r="AI166">
+        <v>208.14667010505994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "with the correct mean annual precipitation"
This reverts commit 2cd023b2c3733aa4400671e3247beb95e548768e.
</commit_message>
<xml_diff>
--- a/with climate data and WWTP coordinate.xlsx
+++ b/with climate data and WWTP coordinate.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bundled!$Z$1:$Z$166</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -959,10 +959,10 @@
     <t>Longtitude</t>
   </si>
   <si>
+    <t>mean annual precipitation (mm)</t>
+  </si>
+  <si>
     <t>mean annual temperature (celsius degree)</t>
-  </si>
-  <si>
-    <t>mean annual precipitation (mm)</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1299,8 @@
   <dimension ref="A1:AI166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ6" sqref="AJ6"/>
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1315,7 @@
     <col min="32" max="32" width="11" style="2"/>
     <col min="33" max="33" width="46.625" style="2" customWidth="1"/>
     <col min="34" max="34" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.25" customWidth="1"/>
+    <col min="35" max="35" width="30.75" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -1419,10 +1419,10 @@
         <v>307</v>
       </c>
       <c r="AH1" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1525,8 +1525,8 @@
       <c r="AH2" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI2">
-        <v>482.52000884711742</v>
+      <c r="AI2" s="5">
+        <v>402.10000737259782</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -1629,8 +1629,8 @@
       <c r="AH3" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI3">
-        <v>482.52000884711742</v>
+      <c r="AI3" s="5">
+        <v>402.10000737259782</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1733,8 +1733,8 @@
       <c r="AH4" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI4">
-        <v>482.52000884711742</v>
+      <c r="AI4" s="5">
+        <v>402.10000737259782</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1837,8 +1837,8 @@
       <c r="AH5" s="5">
         <v>12.141944655051661</v>
       </c>
-      <c r="AI5">
-        <v>467.22000859454272</v>
+      <c r="AI5" s="5">
+        <v>389.35000716211897</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1941,8 +1941,8 @@
       <c r="AH6" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI6">
-        <v>1264.0833567380905</v>
+      <c r="AI6" s="5">
+        <v>1053.4027972817421</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -2045,8 +2045,8 @@
       <c r="AH7" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI7">
-        <v>1227.7666888475419</v>
+      <c r="AI7" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -2149,8 +2149,8 @@
       <c r="AH8" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI8">
-        <v>1227.7666888475419</v>
+      <c r="AI8" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
@@ -2253,8 +2253,8 @@
       <c r="AH9" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI9">
-        <v>1227.7666888475419</v>
+      <c r="AI9" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -2357,8 +2357,8 @@
       <c r="AH10" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI10">
-        <v>1227.7666888475419</v>
+      <c r="AI10" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -2461,8 +2461,8 @@
       <c r="AH11" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI11">
-        <v>1227.7666888475419</v>
+      <c r="AI11" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -2565,8 +2565,8 @@
       <c r="AH12" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI12">
-        <v>1227.7666888475419</v>
+      <c r="AI12" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -2669,8 +2669,8 @@
       <c r="AH13" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI13">
-        <v>1227.7666888475419</v>
+      <c r="AI13" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -2773,8 +2773,8 @@
       <c r="AH14" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI14">
-        <v>1227.7666888475419</v>
+      <c r="AI14" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -2877,8 +2877,8 @@
       <c r="AH15" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI15">
-        <v>1227.7666888475419</v>
+      <c r="AI15" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -2981,8 +2981,8 @@
       <c r="AH16" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI16">
-        <v>1306.2633549531301</v>
+      <c r="AI16" s="5">
+        <v>1088.552795794275</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -3085,8 +3085,8 @@
       <c r="AH17" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI17">
-        <v>1227.7666888475419</v>
+      <c r="AI17" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
@@ -3189,8 +3189,8 @@
       <c r="AH18" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI18">
-        <v>1227.7666888475419</v>
+      <c r="AI18" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -3293,8 +3293,8 @@
       <c r="AH19" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI19">
-        <v>1306.2633549531301</v>
+      <c r="AI19" s="5">
+        <v>1088.552795794275</v>
       </c>
     </row>
     <row r="20" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3397,8 +3397,8 @@
       <c r="AH20" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI20">
-        <v>1264.0833567380905</v>
+      <c r="AI20" s="5">
+        <v>1053.4027972817421</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -3501,8 +3501,8 @@
       <c r="AH21" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI21">
-        <v>1227.7666888475419</v>
+      <c r="AI21" s="5">
+        <v>1023.1389073729515</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -3605,8 +3605,8 @@
       <c r="AH22" s="5">
         <v>13.163889099905889</v>
       </c>
-      <c r="AI22">
-        <v>489.91334197868906</v>
+      <c r="AI22" s="5">
+        <v>408.26111831557421</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -3709,8 +3709,8 @@
       <c r="AH23" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI23">
-        <v>1152.1833533684412</v>
+      <c r="AI23" s="5">
+        <v>960.15279447370108</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
@@ -3813,8 +3813,8 @@
       <c r="AH24" s="5">
         <v>17.651111385557385</v>
       </c>
-      <c r="AI24">
-        <v>1146.9466877460479</v>
+      <c r="AI24" s="5">
+        <v>955.78890645503998</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -3917,8 +3917,8 @@
       <c r="AH25" s="5">
         <v>15.193055835366248</v>
       </c>
-      <c r="AI25">
-        <v>1171.4066875537237</v>
+      <c r="AI25" s="5">
+        <v>976.17223962810294</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -4021,8 +4021,8 @@
       <c r="AH26" s="5">
         <v>14.228333567414019</v>
       </c>
-      <c r="AI26">
-        <v>1074.7333531796933</v>
+      <c r="AI26" s="5">
+        <v>895.61112764974439</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -4125,8 +4125,8 @@
       <c r="AH27" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI27">
-        <v>1152.1833533684412</v>
+      <c r="AI27" s="5">
+        <v>960.15279447370108</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -4229,8 +4229,8 @@
       <c r="AH28" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI28">
-        <v>1096.6566830794015</v>
+      <c r="AI28" s="5">
+        <v>913.88056923283466</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -4333,8 +4333,8 @@
       <c r="AH29" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI29">
-        <v>1096.6566830794015</v>
+      <c r="AI29" s="5">
+        <v>913.88056923283466</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -4437,8 +4437,8 @@
       <c r="AH30" s="5">
         <v>15.2763891518116</v>
       </c>
-      <c r="AI30">
-        <v>1093.6533483068149</v>
+      <c r="AI30" s="5">
+        <v>911.37779025567909</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
@@ -4541,8 +4541,8 @@
       <c r="AH31" s="5">
         <v>15.491389160023795</v>
       </c>
-      <c r="AI31">
-        <v>1143.6800213019053</v>
+      <c r="AI31" s="5">
+        <v>953.06668441825434</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -4645,8 +4645,8 @@
       <c r="AH32" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI32">
-        <v>1143.4166879415511</v>
+      <c r="AI32" s="5">
+        <v>952.84723995129275</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
@@ -4749,8 +4749,8 @@
       <c r="AH33" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI33">
-        <v>1143.4166879415511</v>
+      <c r="AI33" s="5">
+        <v>952.84723995129275</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
@@ -4853,8 +4853,8 @@
       <c r="AH34" s="5">
         <v>14.283055821309487</v>
       </c>
-      <c r="AI34">
-        <v>1064.9600166936716</v>
+      <c r="AI34" s="5">
+        <v>887.4666805780596</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
@@ -4957,8 +4957,8 @@
       <c r="AH35" s="5">
         <v>16.284166936079661</v>
       </c>
-      <c r="AI35">
-        <v>1184.4866863250732</v>
+      <c r="AI35" s="5">
+        <v>987.07223860422778</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
@@ -5061,8 +5061,8 @@
       <c r="AH36" s="5">
         <v>18.087500296698675</v>
       </c>
-      <c r="AI36">
-        <v>1125.8433512528738</v>
+      <c r="AI36" s="5">
+        <v>938.20279271072809</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
@@ -5165,8 +5165,8 @@
       <c r="AH37" s="5">
         <v>14.717222467395995</v>
       </c>
-      <c r="AI37">
-        <v>1169.6400195121764</v>
+      <c r="AI37" s="5">
+        <v>974.70001626014709</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
@@ -5272,8 +5272,8 @@
       <c r="AH38" s="5">
         <v>13.463055785890255</v>
       </c>
-      <c r="AI38">
-        <v>495.19334186911584</v>
+      <c r="AI38" s="5">
+        <v>412.66111822426319</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
@@ -5379,8 +5379,8 @@
       <c r="AH39" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI39">
-        <v>497.82334056297935</v>
+      <c r="AI39" s="5">
+        <v>414.8527838024828</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
@@ -5486,8 +5486,8 @@
       <c r="AH40" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI40">
-        <v>497.82334056297935</v>
+      <c r="AI40" s="5">
+        <v>414.8527838024828</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
@@ -5593,8 +5593,8 @@
       <c r="AH41" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI41">
-        <v>497.82334056297935</v>
+      <c r="AI41" s="5">
+        <v>414.8527838024828</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
@@ -5700,8 +5700,8 @@
       <c r="AH42" s="5">
         <v>12.47416684911069</v>
       </c>
-      <c r="AI42">
-        <v>511.87667389387883</v>
+      <c r="AI42" s="5">
+        <v>426.56389491156574</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
@@ -5807,8 +5807,8 @@
       <c r="AH43" s="5">
         <v>10.801666868146922</v>
       </c>
-      <c r="AI43">
-        <v>510.76001007730764</v>
+      <c r="AI43" s="5">
+        <v>425.63334173108967</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
@@ -5914,8 +5914,8 @@
       <c r="AH44" s="5">
         <v>14.008333571544952</v>
       </c>
-      <c r="AI44">
-        <v>550.76667751148341</v>
+      <c r="AI44" s="5">
+        <v>458.97223125956953</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
@@ -6021,8 +6021,8 @@
       <c r="AH45" s="5">
         <v>7.1547223484764499</v>
       </c>
-      <c r="AI45">
-        <v>389.3833411594232</v>
+      <c r="AI45" s="5">
+        <v>324.48611763285265</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.25">
@@ -6128,8 +6128,8 @@
       <c r="AH46" s="5">
         <v>6.6944445381975832</v>
       </c>
-      <c r="AI46">
-        <v>344.61333842054012</v>
+      <c r="AI46" s="5">
+        <v>287.17778201711673</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
@@ -6235,8 +6235,8 @@
       <c r="AH47" s="5">
         <v>4.4341667553409936</v>
       </c>
-      <c r="AI47">
-        <v>514.92334158072867</v>
+      <c r="AI47" s="5">
+        <v>429.1027846506073</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.25">
@@ -6342,8 +6342,8 @@
       <c r="AH48" s="5">
         <v>4.5591666952189476</v>
       </c>
-      <c r="AI48">
-        <v>422.96667394911248</v>
+      <c r="AI48" s="5">
+        <v>352.47222829092709</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.25">
@@ -6449,8 +6449,8 @@
       <c r="AH49" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI49">
-        <v>702.19001223693294</v>
+      <c r="AI49" s="5">
+        <v>585.15834353077742</v>
       </c>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.25">
@@ -6556,8 +6556,8 @@
       <c r="AH50" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI50">
-        <v>669.66001015752556</v>
+      <c r="AI50" s="5">
+        <v>558.05000846460462</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.25">
@@ -6663,8 +6663,8 @@
       <c r="AH51" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI51">
-        <v>669.66001015752556</v>
+      <c r="AI51" s="5">
+        <v>558.05000846460462</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.25">
@@ -6770,8 +6770,8 @@
       <c r="AH52" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI52">
-        <v>669.66001015752556</v>
+      <c r="AI52" s="5">
+        <v>558.05000846460462</v>
       </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
@@ -6877,8 +6877,8 @@
       <c r="AH53" s="5">
         <v>11.009722441848782</v>
       </c>
-      <c r="AI53">
-        <v>628.88001114701228</v>
+      <c r="AI53" s="5">
+        <v>524.06667595584361</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
@@ -6984,8 +6984,8 @@
       <c r="AH54" s="5">
         <v>9.6700001836236975</v>
       </c>
-      <c r="AI54">
-        <v>662.87001019318893</v>
+      <c r="AI54" s="5">
+        <v>552.39167516099076</v>
       </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.25">
@@ -7091,8 +7091,8 @@
       <c r="AH55" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI55">
-        <v>702.19001223693294</v>
+      <c r="AI55" s="5">
+        <v>585.15834353077742</v>
       </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.25">
@@ -7198,8 +7198,8 @@
       <c r="AH56" s="5">
         <v>7.8900001508080297</v>
       </c>
-      <c r="AI56">
-        <v>646.52667742843425</v>
+      <c r="AI56" s="5">
+        <v>538.77223119036194</v>
       </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.25">
@@ -7305,8 +7305,8 @@
       <c r="AH57" s="5">
         <v>5.0902778515799181</v>
       </c>
-      <c r="AI57">
-        <v>436.14334103912114</v>
+      <c r="AI57" s="5">
+        <v>363.45278419926763</v>
       </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
@@ -7412,8 +7412,8 @@
       <c r="AH58" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI58">
-        <v>687.9300124709805</v>
+      <c r="AI58" s="5">
+        <v>573.27501039248375</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.25">
@@ -7519,8 +7519,8 @@
       <c r="AH59" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI59">
-        <v>687.9300124709805</v>
+      <c r="AI59" s="5">
+        <v>573.27501039248375</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.25">
@@ -7626,8 +7626,8 @@
       <c r="AH60" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI60">
-        <v>687.9300124709805</v>
+      <c r="AI60" s="5">
+        <v>573.27501039248375</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.25">
@@ -7733,8 +7733,8 @@
       <c r="AH61" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI61">
-        <v>687.9300124709805</v>
+      <c r="AI61" s="5">
+        <v>573.27501039248375</v>
       </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
@@ -7840,8 +7840,8 @@
       <c r="AH62" s="5">
         <v>12.402500250997642</v>
       </c>
-      <c r="AI62">
-        <v>656.74667675495152</v>
+      <c r="AI62" s="5">
+        <v>547.28889729579282</v>
       </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.25">
@@ -7947,8 +7947,8 @@
       <c r="AH63" s="5">
         <v>13.197500290266342</v>
       </c>
-      <c r="AI63">
-        <v>656.12001041024928</v>
+      <c r="AI63" s="5">
+        <v>546.76667534187436</v>
       </c>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.25">
@@ -8054,8 +8054,8 @@
       <c r="AH64" s="5">
         <v>14.578889134505557</v>
       </c>
-      <c r="AI64">
-        <v>783.4933441119889</v>
+      <c r="AI64" s="5">
+        <v>652.91112009332414</v>
       </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.25">
@@ -8161,8 +8161,8 @@
       <c r="AH65" s="5">
         <v>11.883889088572728</v>
       </c>
-      <c r="AI65">
-        <v>683.65334561069801</v>
+      <c r="AI65" s="5">
+        <v>569.71112134224836</v>
       </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.25">
@@ -8268,8 +8268,8 @@
       <c r="AH66" s="5">
         <v>12.213611334106988</v>
       </c>
-      <c r="AI66">
-        <v>630.5100109905004</v>
+      <c r="AI66" s="5">
+        <v>525.42500915875041</v>
       </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.25">
@@ -8375,8 +8375,8 @@
       <c r="AH67" s="5">
         <v>13.395278038394947</v>
       </c>
-      <c r="AI67">
-        <v>644.73334439744553</v>
+      <c r="AI67" s="5">
+        <v>537.2777869978712</v>
       </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.25">
@@ -8482,8 +8482,8 @@
       <c r="AH68" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI68">
-        <v>679.74667786136274</v>
+      <c r="AI68" s="5">
+        <v>566.45556488446891</v>
       </c>
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.25">
@@ -8589,8 +8589,8 @@
       <c r="AH69" s="5">
         <v>14.514166940645211</v>
       </c>
-      <c r="AI69">
-        <v>715.4333448857069</v>
+      <c r="AI69" s="5">
+        <v>596.19445407142246</v>
       </c>
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.25">
@@ -8696,8 +8696,8 @@
       <c r="AH70" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI70">
-        <v>679.74667786136274</v>
+      <c r="AI70" s="5">
+        <v>566.45556488446891</v>
       </c>
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.25">
@@ -8803,8 +8803,8 @@
       <c r="AH71" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI71">
-        <v>679.74667786136274</v>
+      <c r="AI71" s="5">
+        <v>566.45556488446891</v>
       </c>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.25">
@@ -8910,8 +8910,8 @@
       <c r="AH72" s="5">
         <v>13.200278020401795</v>
       </c>
-      <c r="AI72">
-        <v>684.12334228530528</v>
+      <c r="AI72" s="5">
+        <v>570.10278523775446</v>
       </c>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.25">
@@ -9017,8 +9017,8 @@
       <c r="AH73" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI73">
-        <v>744.21001186221838</v>
+      <c r="AI73" s="5">
+        <v>620.17500988518202</v>
       </c>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.25">
@@ -9124,8 +9124,8 @@
       <c r="AH74" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI74">
-        <v>744.21001186221838</v>
+      <c r="AI74" s="5">
+        <v>620.17500988518202</v>
       </c>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.25">
@@ -9231,8 +9231,8 @@
       <c r="AH75" s="5">
         <v>12.714166869243813</v>
       </c>
-      <c r="AI75">
-        <v>724.0633454682926</v>
+      <c r="AI75" s="5">
+        <v>603.38612122357722</v>
       </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.25">
@@ -9338,8 +9338,8 @@
       <c r="AH76" s="5">
         <v>14.380278021987113</v>
       </c>
-      <c r="AI76">
-        <v>590.31334434126813</v>
+      <c r="AI76" s="5">
+        <v>491.92778695105682</v>
       </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.25">
@@ -9445,8 +9445,8 @@
       <c r="AH77" s="5">
         <v>15.016111336586375</v>
       </c>
-      <c r="AI77">
-        <v>628.21667590836682</v>
+      <c r="AI77" s="5">
+        <v>523.51389659030576</v>
       </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.25">
@@ -9552,8 +9552,8 @@
       <c r="AH78" s="5">
         <v>14.131666897899574</v>
       </c>
-      <c r="AI78">
-        <v>730.94001448949177</v>
+      <c r="AI78" s="5">
+        <v>609.11667874124316</v>
       </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.25">
@@ -9659,8 +9659,8 @@
       <c r="AH79" s="5">
         <v>14.880833575605518</v>
       </c>
-      <c r="AI79">
-        <v>670.98001096273458</v>
+      <c r="AI79" s="5">
+        <v>559.15000913561221</v>
       </c>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.25">
@@ -9766,8 +9766,8 @@
       <c r="AH80" s="5">
         <v>16.243055798009866</v>
       </c>
-      <c r="AI80">
-        <v>1169.4566881649196</v>
+      <c r="AI80" s="5">
+        <v>974.54724013743305</v>
       </c>
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.25">
@@ -9873,8 +9873,8 @@
       <c r="AH81" s="5">
         <v>16.389166925619875</v>
       </c>
-      <c r="AI81">
-        <v>1255.1900207134584</v>
+      <c r="AI81" s="5">
+        <v>1045.9916839278819</v>
       </c>
     </row>
     <row r="82" spans="1:35" x14ac:dyDescent="0.25">
@@ -9980,8 +9980,8 @@
       <c r="AH82" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI82">
-        <v>1167.3833518219492</v>
+      <c r="AI82" s="5">
+        <v>972.81945985162429</v>
       </c>
     </row>
     <row r="83" spans="1:35" x14ac:dyDescent="0.25">
@@ -10087,8 +10087,8 @@
       <c r="AH83" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI83">
-        <v>1167.3833518219492</v>
+      <c r="AI83" s="5">
+        <v>972.81945985162429</v>
       </c>
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.25">
@@ -10194,8 +10194,8 @@
       <c r="AH84" s="5">
         <v>15.054166897386313</v>
       </c>
-      <c r="AI84">
-        <v>816.7133487234513</v>
+      <c r="AI84" s="5">
+        <v>680.59445726954277</v>
       </c>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.25">
@@ -10301,8 +10301,8 @@
       <c r="AH85" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI85">
-        <v>1171.370017160227</v>
+      <c r="AI85" s="5">
+        <v>976.1416809668558</v>
       </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.25">
@@ -10408,8 +10408,8 @@
       <c r="AH86" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI86">
-        <v>1171.370017160227</v>
+      <c r="AI86" s="5">
+        <v>976.1416809668558</v>
       </c>
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.25">
@@ -10515,8 +10515,8 @@
       <c r="AH87" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI87">
-        <v>1171.370017160227</v>
+      <c r="AI87" s="5">
+        <v>976.1416809668558</v>
       </c>
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.25">
@@ -10622,8 +10622,8 @@
       <c r="AH88" s="5">
         <v>16.396111346284549</v>
       </c>
-      <c r="AI88">
-        <v>1227.8800224574904</v>
+      <c r="AI88" s="5">
+        <v>1023.2333520479086</v>
       </c>
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.25">
@@ -10729,8 +10729,8 @@
       <c r="AH89" s="5">
         <v>15.944722454353339</v>
       </c>
-      <c r="AI89">
-        <v>1167.9366861462593</v>
+      <c r="AI89" s="5">
+        <v>973.28057178854942</v>
       </c>
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.25">
@@ -10836,8 +10836,8 @@
       <c r="AH90" s="5">
         <v>15.40638912299441</v>
       </c>
-      <c r="AI90">
-        <v>1124.8166836957137</v>
+      <c r="AI90" s="5">
+        <v>937.34723641309472</v>
       </c>
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.25">
@@ -10943,8 +10943,8 @@
       <c r="AH91" s="5">
         <v>14.980833584670391</v>
       </c>
-      <c r="AI91">
-        <v>906.1300134827693</v>
+      <c r="AI91" s="5">
+        <v>755.10834456897442</v>
       </c>
     </row>
     <row r="92" spans="1:35" x14ac:dyDescent="0.25">
@@ -11050,8 +11050,8 @@
       <c r="AH92" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI92">
-        <v>1100.000017362833</v>
+      <c r="AI92" s="5">
+        <v>916.66668113569415</v>
       </c>
     </row>
     <row r="93" spans="1:35" x14ac:dyDescent="0.25">
@@ -11157,8 +11157,8 @@
       <c r="AH93" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI93">
-        <v>1100.000017362833</v>
+      <c r="AI93" s="5">
+        <v>916.66668113569415</v>
       </c>
     </row>
     <row r="94" spans="1:35" x14ac:dyDescent="0.25">
@@ -11264,8 +11264,8 @@
       <c r="AH94" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI94">
-        <v>1171.370017160227</v>
+      <c r="AI94" s="5">
+        <v>976.1416809668558</v>
       </c>
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.25">
@@ -11371,8 +11371,8 @@
       <c r="AH95" s="5">
         <v>15.691944675313103</v>
       </c>
-      <c r="AI95">
-        <v>1101.9933541138967</v>
+      <c r="AI95" s="5">
+        <v>918.32779509491388</v>
       </c>
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.25">
@@ -11478,8 +11478,8 @@
       <c r="AH96" s="5">
         <v>15.582500197138224</v>
       </c>
-      <c r="AI96">
-        <v>853.43668373152616</v>
+      <c r="AI96" s="5">
+        <v>711.19723644293845</v>
       </c>
     </row>
     <row r="97" spans="1:35" x14ac:dyDescent="0.25">
@@ -11585,8 +11585,8 @@
       <c r="AH97" s="5">
         <v>16.058055824786425</v>
       </c>
-      <c r="AI97">
-        <v>970.44001293977101</v>
+      <c r="AI97" s="5">
+        <v>808.70001078314249</v>
       </c>
     </row>
     <row r="98" spans="1:35" x14ac:dyDescent="0.25">
@@ -11692,8 +11692,8 @@
       <c r="AH98" s="5">
         <v>15.946111321780418</v>
       </c>
-      <c r="AI98">
-        <v>996.45668524280188</v>
+      <c r="AI98" s="5">
+        <v>830.38057103566825</v>
       </c>
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.25">
@@ -11799,8 +11799,8 @@
       <c r="AH99" s="5">
         <v>16.454722446203231</v>
       </c>
-      <c r="AI99">
-        <v>1158.6466879757743</v>
+      <c r="AI99" s="5">
+        <v>965.53890664647849</v>
       </c>
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.25">
@@ -11906,8 +11906,8 @@
       <c r="AH100" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI100">
-        <v>1412.5500238403679</v>
+      <c r="AI100" s="5">
+        <v>1177.1250198669732</v>
       </c>
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.25">
@@ -12013,8 +12013,8 @@
       <c r="AH101" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI101">
-        <v>1412.5500238403679</v>
+      <c r="AI101" s="5">
+        <v>1177.1250198669732</v>
       </c>
     </row>
     <row r="102" spans="1:35" x14ac:dyDescent="0.25">
@@ -12120,8 +12120,8 @@
       <c r="AH102" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI102">
-        <v>1412.5500238403679</v>
+      <c r="AI102" s="5">
+        <v>1177.1250198669732</v>
       </c>
     </row>
     <row r="103" spans="1:35" x14ac:dyDescent="0.25">
@@ -12227,8 +12227,8 @@
       <c r="AH103" s="5">
         <v>15.962500282625358</v>
       </c>
-      <c r="AI103">
-        <v>1501.7400254786014</v>
+      <c r="AI103" s="5">
+        <v>1251.4500212321677</v>
       </c>
     </row>
     <row r="104" spans="1:35" x14ac:dyDescent="0.25">
@@ -12334,8 +12334,8 @@
       <c r="AH104" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI104">
-        <v>1429.3566899955272</v>
+      <c r="AI104" s="5">
+        <v>1191.1305749962728</v>
       </c>
     </row>
     <row r="105" spans="1:35" x14ac:dyDescent="0.25">
@@ -12441,8 +12441,8 @@
       <c r="AH105" s="5">
         <v>17.36972248951594</v>
       </c>
-      <c r="AI105">
-        <v>1619.7266931096713</v>
+      <c r="AI105" s="5">
+        <v>1349.7722442580593</v>
       </c>
     </row>
     <row r="106" spans="1:35" x14ac:dyDescent="0.25">
@@ -12548,8 +12548,8 @@
       <c r="AH106" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI106">
-        <v>1429.3566899955272</v>
+      <c r="AI106" s="5">
+        <v>1191.1305749962728</v>
       </c>
     </row>
     <row r="107" spans="1:35" x14ac:dyDescent="0.25">
@@ -12655,8 +12655,8 @@
       <c r="AH107" s="5">
         <v>16.991666977935367</v>
       </c>
-      <c r="AI107">
-        <v>1461.4566946188609</v>
+      <c r="AI107" s="5">
+        <v>1217.8805788490508</v>
       </c>
     </row>
     <row r="108" spans="1:35" x14ac:dyDescent="0.25">
@@ -12762,8 +12762,8 @@
       <c r="AH108" s="5">
         <v>17.177500254909198</v>
       </c>
-      <c r="AI108">
-        <v>1376.8500243378182</v>
+      <c r="AI108" s="5">
+        <v>1147.3750202815152</v>
       </c>
     </row>
     <row r="109" spans="1:35" x14ac:dyDescent="0.25">
@@ -12869,8 +12869,8 @@
       <c r="AH109" s="5">
         <v>16.59805584020085</v>
       </c>
-      <c r="AI109">
-        <v>1607.316695245107</v>
+      <c r="AI109" s="5">
+        <v>1339.4305793709225</v>
       </c>
     </row>
     <row r="110" spans="1:35" x14ac:dyDescent="0.25">
@@ -12976,8 +12976,8 @@
       <c r="AH110" s="5">
         <v>18.400555811987982</v>
       </c>
-      <c r="AI110">
-        <v>1670.273362938563</v>
+      <c r="AI110" s="5">
+        <v>1391.8944691154693</v>
       </c>
     </row>
     <row r="111" spans="1:35" x14ac:dyDescent="0.25">
@@ -13083,8 +13083,8 @@
       <c r="AH111" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI111">
-        <v>1325.3133495601514</v>
+      <c r="AI111" s="5">
+        <v>1104.4277913001263</v>
       </c>
     </row>
     <row r="112" spans="1:35" x14ac:dyDescent="0.25">
@@ -13190,8 +13190,8 @@
       <c r="AH112" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI112">
-        <v>1325.3133495601514</v>
+      <c r="AI112" s="5">
+        <v>1104.4277913001263</v>
       </c>
     </row>
     <row r="113" spans="1:35" x14ac:dyDescent="0.25">
@@ -13297,8 +13297,8 @@
       <c r="AH113" s="5">
         <v>16.237500274015797</v>
       </c>
-      <c r="AI113">
-        <v>1339.0533566698432</v>
+      <c r="AI113" s="5">
+        <v>1115.8777972248693</v>
       </c>
     </row>
     <row r="114" spans="1:35" x14ac:dyDescent="0.25">
@@ -13404,8 +13404,8 @@
       <c r="AH114" s="5">
         <v>16.611111394564311</v>
       </c>
-      <c r="AI114">
-        <v>1451.9166888972125</v>
+      <c r="AI114" s="5">
+        <v>1209.9305740810103</v>
       </c>
     </row>
     <row r="115" spans="1:35" x14ac:dyDescent="0.25">
@@ -13511,8 +13511,8 @@
       <c r="AH115" s="5">
         <v>16.962222494681676</v>
       </c>
-      <c r="AI115">
-        <v>1551.293354121844</v>
+      <c r="AI115" s="5">
+        <v>1292.7444617682033</v>
       </c>
     </row>
     <row r="116" spans="1:35" x14ac:dyDescent="0.25">
@@ -13618,8 +13618,8 @@
       <c r="AH116" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI116">
-        <v>1504.2333610216776</v>
+      <c r="AI116" s="5">
+        <v>1253.5278008513981</v>
       </c>
     </row>
     <row r="117" spans="1:35" x14ac:dyDescent="0.25">
@@ -13725,8 +13725,8 @@
       <c r="AH117" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI117">
-        <v>1504.2333610216776</v>
+      <c r="AI117" s="5">
+        <v>1253.5278008513981</v>
       </c>
     </row>
     <row r="118" spans="1:35" x14ac:dyDescent="0.25">
@@ -13832,8 +13832,8 @@
       <c r="AH118" s="5">
         <v>17.300555813312531</v>
       </c>
-      <c r="AI118">
-        <v>1707.6833669265111</v>
+      <c r="AI118" s="5">
+        <v>1423.0694724387592</v>
       </c>
     </row>
     <row r="119" spans="1:35" x14ac:dyDescent="0.25">
@@ -13939,8 +13939,8 @@
       <c r="AH119" s="5">
         <v>16.892500269412995</v>
       </c>
-      <c r="AI119">
-        <v>1603.7033581415812</v>
+      <c r="AI119" s="5">
+        <v>1336.4194651179844</v>
       </c>
     </row>
     <row r="120" spans="1:35" x14ac:dyDescent="0.25">
@@ -14046,8 +14046,8 @@
       <c r="AH120" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI120">
-        <v>1540.4100324869155</v>
+      <c r="AI120" s="5">
+        <v>1283.6750270724297</v>
       </c>
     </row>
     <row r="121" spans="1:35" x14ac:dyDescent="0.25">
@@ -14153,8 +14153,8 @@
       <c r="AH121" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI121">
-        <v>1540.4100324869155</v>
+      <c r="AI121" s="5">
+        <v>1283.6750270724297</v>
       </c>
     </row>
     <row r="122" spans="1:35" x14ac:dyDescent="0.25">
@@ -14260,8 +14260,8 @@
       <c r="AH122" s="5">
         <v>17.377222496933406</v>
       </c>
-      <c r="AI122">
-        <v>1612.0533617973329</v>
+      <c r="AI122" s="5">
+        <v>1343.3778014977772</v>
       </c>
     </row>
     <row r="123" spans="1:35" x14ac:dyDescent="0.25">
@@ -14367,8 +14367,8 @@
       <c r="AH123" s="5">
         <v>18.61972255706787</v>
       </c>
-      <c r="AI123">
-        <v>1583.2933620850245</v>
+      <c r="AI123" s="5">
+        <v>1319.411135070854</v>
       </c>
     </row>
     <row r="124" spans="1:35" x14ac:dyDescent="0.25">
@@ -14474,8 +14474,8 @@
       <c r="AH124" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI124">
-        <v>1782.6833617116015</v>
+      <c r="AI124" s="5">
+        <v>1485.5694680930012</v>
       </c>
     </row>
     <row r="125" spans="1:35" x14ac:dyDescent="0.25">
@@ -14581,8 +14581,8 @@
       <c r="AH125" s="5">
         <v>21.330278105205959</v>
       </c>
-      <c r="AI125">
-        <v>1417.5933627367019</v>
+      <c r="AI125" s="5">
+        <v>1181.3278022805848</v>
       </c>
     </row>
     <row r="126" spans="1:35" x14ac:dyDescent="0.25">
@@ -14688,8 +14688,8 @@
       <c r="AH126" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI126">
-        <v>1782.6833617116015</v>
+      <c r="AI126" s="5">
+        <v>1485.5694680930012</v>
       </c>
     </row>
     <row r="127" spans="1:35" x14ac:dyDescent="0.25">
@@ -14795,8 +14795,8 @@
       <c r="AH127" s="5">
         <v>14.705277992950545</v>
       </c>
-      <c r="AI127">
-        <v>654.54667957797642</v>
+      <c r="AI127" s="5">
+        <v>545.45556631498039</v>
       </c>
     </row>
     <row r="128" spans="1:35" x14ac:dyDescent="0.25">
@@ -14902,8 +14902,8 @@
       <c r="AH128" s="5">
         <v>15.146666885043183</v>
       </c>
-      <c r="AI128">
-        <v>613.37334387948113</v>
+      <c r="AI128" s="5">
+        <v>511.14445323290101</v>
       </c>
     </row>
     <row r="129" spans="1:35" x14ac:dyDescent="0.25">
@@ -15009,8 +15009,8 @@
       <c r="AH129" s="5">
         <v>15.114166894327436</v>
       </c>
-      <c r="AI129">
-        <v>663.24001225084066</v>
+      <c r="AI129" s="5">
+        <v>552.70001020903385</v>
       </c>
     </row>
     <row r="130" spans="1:35" x14ac:dyDescent="0.25">
@@ -15116,8 +15116,8 @@
       <c r="AH130" s="5">
         <v>14.685000222010745</v>
       </c>
-      <c r="AI130">
-        <v>619.34667505845425</v>
+      <c r="AI130" s="5">
+        <v>516.12222921537852</v>
       </c>
     </row>
     <row r="131" spans="1:35" x14ac:dyDescent="0.25">
@@ -15223,8 +15223,8 @@
       <c r="AH131" s="5">
         <v>14.560555819484096</v>
       </c>
-      <c r="AI131">
-        <v>583.81001118198037</v>
+      <c r="AI131" s="5">
+        <v>486.50834265165031</v>
       </c>
     </row>
     <row r="132" spans="1:35" x14ac:dyDescent="0.25">
@@ -15330,8 +15330,8 @@
       <c r="AH132" s="5">
         <v>14.925000269276401</v>
       </c>
-      <c r="AI132">
-        <v>705.52334533234432</v>
+      <c r="AI132" s="5">
+        <v>587.93612111028699</v>
       </c>
     </row>
     <row r="133" spans="1:35" x14ac:dyDescent="0.25">
@@ -15437,8 +15437,8 @@
       <c r="AH133" s="5">
         <v>14.240833549056616</v>
       </c>
-      <c r="AI133">
-        <v>694.26334502796328</v>
+      <c r="AI133" s="5">
+        <v>578.55278752330275</v>
       </c>
     </row>
     <row r="134" spans="1:35" x14ac:dyDescent="0.25">
@@ -15544,8 +15544,8 @@
       <c r="AH134" s="5">
         <v>15.481111367895371</v>
       </c>
-      <c r="AI134">
-        <v>796.98001470267775</v>
+      <c r="AI134" s="5">
+        <v>664.15001225223148</v>
       </c>
     </row>
     <row r="135" spans="1:35" x14ac:dyDescent="0.25">
@@ -15651,8 +15651,8 @@
       <c r="AH135" s="5">
         <v>15.808611411021815</v>
       </c>
-      <c r="AI135">
-        <v>878.90668233633039</v>
+      <c r="AI135" s="5">
+        <v>732.42223528027534</v>
       </c>
     </row>
     <row r="136" spans="1:35" x14ac:dyDescent="0.25">
@@ -15758,8 +15758,8 @@
       <c r="AH136" s="5">
         <v>16.348055789868038</v>
       </c>
-      <c r="AI136">
-        <v>847.81001371790967</v>
+      <c r="AI136" s="5">
+        <v>706.5083447649248</v>
       </c>
     </row>
     <row r="137" spans="1:35" x14ac:dyDescent="0.25">
@@ -15865,8 +15865,8 @@
       <c r="AH137" s="5">
         <v>13.885278014466166</v>
       </c>
-      <c r="AI137">
-        <v>578.90334290241196</v>
+      <c r="AI137" s="5">
+        <v>482.41945241867666</v>
       </c>
     </row>
     <row r="138" spans="1:35" x14ac:dyDescent="0.25">
@@ -15972,8 +15972,8 @@
       <c r="AH138" s="5">
         <v>17.218055825101004</v>
       </c>
-      <c r="AI138">
-        <v>1247.3300210356713</v>
+      <c r="AI138" s="5">
+        <v>1039.4416841963928</v>
       </c>
     </row>
     <row r="139" spans="1:35" x14ac:dyDescent="0.25">
@@ -16079,8 +16079,8 @@
       <c r="AH139" s="5">
         <v>17.671944708956612</v>
       </c>
-      <c r="AI139">
-        <v>1440.4833574632803</v>
+      <c r="AI139" s="5">
+        <v>1200.402797886067</v>
       </c>
     </row>
     <row r="140" spans="1:35" x14ac:dyDescent="0.25">
@@ -16186,8 +16186,8 @@
       <c r="AH140" s="5">
         <v>17.840000283055836</v>
       </c>
-      <c r="AI140">
-        <v>1479.7433575078844</v>
+      <c r="AI140" s="5">
+        <v>1233.1194645899038</v>
       </c>
     </row>
     <row r="141" spans="1:35" x14ac:dyDescent="0.25">
@@ -16293,8 +16293,8 @@
       <c r="AH141" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI141">
-        <v>2196.9867067073783</v>
+      <c r="AI141" s="5">
+        <v>1830.8222555894818</v>
       </c>
     </row>
     <row r="142" spans="1:35" x14ac:dyDescent="0.25">
@@ -16400,8 +16400,8 @@
       <c r="AH142" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI142">
-        <v>2196.9867067073783</v>
+      <c r="AI142" s="5">
+        <v>1830.8222555894818</v>
       </c>
     </row>
     <row r="143" spans="1:35" x14ac:dyDescent="0.25">
@@ -16507,8 +16507,8 @@
       <c r="AH143" s="5">
         <v>22.497500356038412</v>
       </c>
-      <c r="AI143">
-        <v>1748.520027906696</v>
+      <c r="AI143" s="5">
+        <v>1457.10002325558</v>
       </c>
     </row>
     <row r="144" spans="1:35" x14ac:dyDescent="0.25">
@@ -16614,8 +16614,8 @@
       <c r="AH144" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI144">
-        <v>1001.1966831016044</v>
+      <c r="AI144" s="5">
+        <v>834.33056925133701</v>
       </c>
     </row>
     <row r="145" spans="1:35" x14ac:dyDescent="0.25">
@@ -16721,8 +16721,8 @@
       <c r="AH145" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI145">
-        <v>1001.1966831016044</v>
+      <c r="AI145" s="5">
+        <v>834.33056925133701</v>
       </c>
     </row>
     <row r="146" spans="1:35" x14ac:dyDescent="0.25">
@@ -16828,8 +16828,8 @@
       <c r="AH146" s="5">
         <v>16.466389189826117</v>
       </c>
-      <c r="AI146">
-        <v>1009.2633496473233</v>
+      <c r="AI146" s="5">
+        <v>841.05279137276943</v>
       </c>
     </row>
     <row r="147" spans="1:35" x14ac:dyDescent="0.25">
@@ -16935,8 +16935,8 @@
       <c r="AH147" s="5">
         <v>18.550555888811747</v>
       </c>
-      <c r="AI147">
-        <v>1105.6566875979304</v>
+      <c r="AI147" s="5">
+        <v>921.3805729982754</v>
       </c>
     </row>
     <row r="148" spans="1:35" x14ac:dyDescent="0.25">
@@ -17042,8 +17042,8 @@
       <c r="AH148" s="5">
         <v>16.811666933695474</v>
       </c>
-      <c r="AI148">
-        <v>927.98334970076883</v>
+      <c r="AI148" s="5">
+        <v>773.31945808397393</v>
       </c>
     </row>
     <row r="149" spans="1:35" x14ac:dyDescent="0.25">
@@ -17149,8 +17149,8 @@
       <c r="AH149" s="5">
         <v>16.939166976345909</v>
       </c>
-      <c r="AI149">
-        <v>983.30335068504019</v>
+      <c r="AI149" s="5">
+        <v>819.41945890420016</v>
       </c>
     </row>
     <row r="150" spans="1:35" x14ac:dyDescent="0.25">
@@ -17256,8 +17256,8 @@
       <c r="AH150" s="5">
         <v>17.050555853048959</v>
       </c>
-      <c r="AI150">
-        <v>1071.2700172980626</v>
+      <c r="AI150" s="5">
+        <v>892.72501441505233</v>
       </c>
     </row>
     <row r="151" spans="1:35" x14ac:dyDescent="0.25">
@@ -17363,8 +17363,8 @@
       <c r="AH151" s="5">
         <v>18.485833643542396</v>
       </c>
-      <c r="AI151">
-        <v>1046.4833499987919</v>
+      <c r="AI151" s="5">
+        <v>872.06945833232669</v>
       </c>
     </row>
     <row r="152" spans="1:35" x14ac:dyDescent="0.25">
@@ -17470,8 +17470,8 @@
       <c r="AH152" s="5">
         <v>17.482500301467049</v>
       </c>
-      <c r="AI152">
-        <v>1032.8100182595351</v>
+      <c r="AI152" s="5">
+        <v>860.67501521627935</v>
       </c>
     </row>
     <row r="153" spans="1:35" x14ac:dyDescent="0.25">
@@ -17577,8 +17577,8 @@
       <c r="AH153" s="5">
         <v>17.544166929192013</v>
       </c>
-      <c r="AI153">
-        <v>1064.7866849660873</v>
+      <c r="AI153" s="5">
+        <v>887.32223747173953</v>
       </c>
     </row>
     <row r="154" spans="1:35" x14ac:dyDescent="0.25">
@@ -17684,8 +17684,8 @@
       <c r="AH154" s="5">
         <v>17.002222526735729</v>
       </c>
-      <c r="AI154">
-        <v>1089.0833561579386</v>
+      <c r="AI154" s="5">
+        <v>907.56946346494885</v>
       </c>
     </row>
     <row r="155" spans="1:35" x14ac:dyDescent="0.25">
@@ -17791,8 +17791,8 @@
       <c r="AH155" s="5">
         <v>16.162500272856818</v>
       </c>
-      <c r="AI155">
-        <v>1124.6000175555548</v>
+      <c r="AI155" s="5">
+        <v>937.16668129629556</v>
       </c>
     </row>
     <row r="156" spans="1:35" x14ac:dyDescent="0.25">
@@ -17898,8 +17898,8 @@
       <c r="AH156" s="5">
         <v>13.510278080569373</v>
       </c>
-      <c r="AI156">
-        <v>945.16001687819755</v>
+      <c r="AI156" s="5">
+        <v>787.63334739849802</v>
       </c>
     </row>
     <row r="157" spans="1:35" x14ac:dyDescent="0.25">
@@ -18005,8 +18005,8 @@
       <c r="AH157" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI157">
-        <v>659.65667902901771</v>
+      <c r="AI157" s="5">
+        <v>549.71389919084811</v>
       </c>
     </row>
     <row r="158" spans="1:35" x14ac:dyDescent="0.25">
@@ -18112,8 +18112,8 @@
       <c r="AH158" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI158">
-        <v>659.65667902901771</v>
+      <c r="AI158" s="5">
+        <v>549.71389919084811</v>
       </c>
     </row>
     <row r="159" spans="1:35" x14ac:dyDescent="0.25">
@@ -18219,8 +18219,8 @@
       <c r="AH159" s="5">
         <v>11.430000214464963</v>
       </c>
-      <c r="AI159">
-        <v>557.09334369699161</v>
+      <c r="AI159" s="5">
+        <v>464.2444530808263</v>
       </c>
     </row>
     <row r="160" spans="1:35" x14ac:dyDescent="0.25">
@@ -18326,8 +18326,8 @@
       <c r="AH160" s="5">
         <v>7.7977779119999875</v>
       </c>
-      <c r="AI160">
-        <v>365.87333956112462</v>
+      <c r="AI160" s="5">
+        <v>304.89444963427053</v>
       </c>
     </row>
     <row r="161" spans="1:35" x14ac:dyDescent="0.25">
@@ -18433,8 +18433,8 @@
       <c r="AH161" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI161">
-        <v>223.68333710978428</v>
+      <c r="AI161" s="5">
+        <v>186.40278092482023</v>
       </c>
     </row>
     <row r="162" spans="1:35" x14ac:dyDescent="0.25">
@@ -18540,8 +18540,8 @@
       <c r="AH162" s="5">
         <v>7.6125001351452539</v>
       </c>
-      <c r="AI162">
-        <v>381.98667274763187</v>
+      <c r="AI162" s="5">
+        <v>318.32222728969322</v>
       </c>
     </row>
     <row r="163" spans="1:35" x14ac:dyDescent="0.25">
@@ -18647,8 +18647,8 @@
       <c r="AH163" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI163">
-        <v>223.68333710978428</v>
+      <c r="AI163" s="5">
+        <v>186.40278092482023</v>
       </c>
     </row>
     <row r="164" spans="1:35" x14ac:dyDescent="0.25">
@@ -18754,8 +18754,8 @@
       <c r="AH164" s="5">
         <v>5.8491667841457655</v>
       </c>
-      <c r="AI164">
-        <v>220.42333756213387</v>
+      <c r="AI164" s="5">
+        <v>183.68611463511155</v>
       </c>
     </row>
     <row r="165" spans="1:35" x14ac:dyDescent="0.25">
@@ -18861,8 +18861,8 @@
       <c r="AH165" s="5">
         <v>4.4586112032747929</v>
       </c>
-      <c r="AI165">
-        <v>232.46667109852035</v>
+      <c r="AI165" s="5">
+        <v>193.72222591543363</v>
       </c>
     </row>
     <row r="166" spans="1:35" x14ac:dyDescent="0.25">
@@ -18968,8 +18968,8 @@
       <c r="AH166" s="5">
         <v>5.5380556673639347</v>
       </c>
-      <c r="AI166">
-        <v>208.14667010505994</v>
+      <c r="AI166" s="5">
+        <v>173.45555842088328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "with the correct mean annual precipitation""
This reverts commit bc3afcde4982185a211b224b52322c236229d6b2.
</commit_message>
<xml_diff>
--- a/with climate data and WWTP coordinate.xlsx
+++ b/with climate data and WWTP coordinate.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bundled!$Z$1:$Z$166</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -959,10 +959,10 @@
     <t>Longtitude</t>
   </si>
   <si>
+    <t>mean annual temperature (celsius degree)</t>
+  </si>
+  <si>
     <t>mean annual precipitation (mm)</t>
-  </si>
-  <si>
-    <t>mean annual temperature (celsius degree)</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1299,8 @@
   <dimension ref="A1:AI166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A1048576"/>
+      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1315,7 @@
     <col min="32" max="32" width="11" style="2"/>
     <col min="33" max="33" width="46.625" style="2" customWidth="1"/>
     <col min="34" max="34" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.75" style="5" customWidth="1"/>
+    <col min="35" max="35" width="30.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -1419,10 +1419,10 @@
         <v>307</v>
       </c>
       <c r="AH1" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AI1" t="s">
         <v>310</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1525,8 +1525,8 @@
       <c r="AH2" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI2" s="5">
-        <v>402.10000737259782</v>
+      <c r="AI2">
+        <v>482.52000884711742</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -1629,8 +1629,8 @@
       <c r="AH3" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI3" s="5">
-        <v>402.10000737259782</v>
+      <c r="AI3">
+        <v>482.52000884711742</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1733,8 +1733,8 @@
       <c r="AH4" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI4" s="5">
-        <v>402.10000737259782</v>
+      <c r="AI4">
+        <v>482.52000884711742</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1837,8 +1837,8 @@
       <c r="AH5" s="5">
         <v>12.141944655051661</v>
       </c>
-      <c r="AI5" s="5">
-        <v>389.35000716211897</v>
+      <c r="AI5">
+        <v>467.22000859454272</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1941,8 +1941,8 @@
       <c r="AH6" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI6" s="5">
-        <v>1053.4027972817421</v>
+      <c r="AI6">
+        <v>1264.0833567380905</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -2045,8 +2045,8 @@
       <c r="AH7" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI7" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI7">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -2149,8 +2149,8 @@
       <c r="AH8" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI8" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI8">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
@@ -2253,8 +2253,8 @@
       <c r="AH9" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI9" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI9">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -2357,8 +2357,8 @@
       <c r="AH10" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI10" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI10">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -2461,8 +2461,8 @@
       <c r="AH11" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI11" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI11">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -2565,8 +2565,8 @@
       <c r="AH12" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI12" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI12">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -2669,8 +2669,8 @@
       <c r="AH13" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI13" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI13">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -2773,8 +2773,8 @@
       <c r="AH14" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI14" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI14">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -2877,8 +2877,8 @@
       <c r="AH15" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI15" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI15">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -2981,8 +2981,8 @@
       <c r="AH16" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI16" s="5">
-        <v>1088.552795794275</v>
+      <c r="AI16">
+        <v>1306.2633549531301</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -3085,8 +3085,8 @@
       <c r="AH17" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI17" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI17">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
@@ -3189,8 +3189,8 @@
       <c r="AH18" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI18" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI18">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -3293,8 +3293,8 @@
       <c r="AH19" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI19" s="5">
-        <v>1088.552795794275</v>
+      <c r="AI19">
+        <v>1306.2633549531301</v>
       </c>
     </row>
     <row r="20" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3397,8 +3397,8 @@
       <c r="AH20" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI20" s="5">
-        <v>1053.4027972817421</v>
+      <c r="AI20">
+        <v>1264.0833567380905</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -3501,8 +3501,8 @@
       <c r="AH21" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI21" s="5">
-        <v>1023.1389073729515</v>
+      <c r="AI21">
+        <v>1227.7666888475419</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -3605,8 +3605,8 @@
       <c r="AH22" s="5">
         <v>13.163889099905889</v>
       </c>
-      <c r="AI22" s="5">
-        <v>408.26111831557421</v>
+      <c r="AI22">
+        <v>489.91334197868906</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -3709,8 +3709,8 @@
       <c r="AH23" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI23" s="5">
-        <v>960.15279447370108</v>
+      <c r="AI23">
+        <v>1152.1833533684412</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
@@ -3813,8 +3813,8 @@
       <c r="AH24" s="5">
         <v>17.651111385557385</v>
       </c>
-      <c r="AI24" s="5">
-        <v>955.78890645503998</v>
+      <c r="AI24">
+        <v>1146.9466877460479</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -3917,8 +3917,8 @@
       <c r="AH25" s="5">
         <v>15.193055835366248</v>
       </c>
-      <c r="AI25" s="5">
-        <v>976.17223962810294</v>
+      <c r="AI25">
+        <v>1171.4066875537237</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -4021,8 +4021,8 @@
       <c r="AH26" s="5">
         <v>14.228333567414019</v>
       </c>
-      <c r="AI26" s="5">
-        <v>895.61112764974439</v>
+      <c r="AI26">
+        <v>1074.7333531796933</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -4125,8 +4125,8 @@
       <c r="AH27" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI27" s="5">
-        <v>960.15279447370108</v>
+      <c r="AI27">
+        <v>1152.1833533684412</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -4229,8 +4229,8 @@
       <c r="AH28" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI28" s="5">
-        <v>913.88056923283466</v>
+      <c r="AI28">
+        <v>1096.6566830794015</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -4333,8 +4333,8 @@
       <c r="AH29" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI29" s="5">
-        <v>913.88056923283466</v>
+      <c r="AI29">
+        <v>1096.6566830794015</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -4437,8 +4437,8 @@
       <c r="AH30" s="5">
         <v>15.2763891518116</v>
       </c>
-      <c r="AI30" s="5">
-        <v>911.37779025567909</v>
+      <c r="AI30">
+        <v>1093.6533483068149</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
@@ -4541,8 +4541,8 @@
       <c r="AH31" s="5">
         <v>15.491389160023795</v>
       </c>
-      <c r="AI31" s="5">
-        <v>953.06668441825434</v>
+      <c r="AI31">
+        <v>1143.6800213019053</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -4645,8 +4645,8 @@
       <c r="AH32" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI32" s="5">
-        <v>952.84723995129275</v>
+      <c r="AI32">
+        <v>1143.4166879415511</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
@@ -4749,8 +4749,8 @@
       <c r="AH33" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI33" s="5">
-        <v>952.84723995129275</v>
+      <c r="AI33">
+        <v>1143.4166879415511</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
@@ -4853,8 +4853,8 @@
       <c r="AH34" s="5">
         <v>14.283055821309487</v>
       </c>
-      <c r="AI34" s="5">
-        <v>887.4666805780596</v>
+      <c r="AI34">
+        <v>1064.9600166936716</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
@@ -4957,8 +4957,8 @@
       <c r="AH35" s="5">
         <v>16.284166936079661</v>
       </c>
-      <c r="AI35" s="5">
-        <v>987.07223860422778</v>
+      <c r="AI35">
+        <v>1184.4866863250732</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
@@ -5061,8 +5061,8 @@
       <c r="AH36" s="5">
         <v>18.087500296698675</v>
       </c>
-      <c r="AI36" s="5">
-        <v>938.20279271072809</v>
+      <c r="AI36">
+        <v>1125.8433512528738</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
@@ -5165,8 +5165,8 @@
       <c r="AH37" s="5">
         <v>14.717222467395995</v>
       </c>
-      <c r="AI37" s="5">
-        <v>974.70001626014709</v>
+      <c r="AI37">
+        <v>1169.6400195121764</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
@@ -5272,8 +5272,8 @@
       <c r="AH38" s="5">
         <v>13.463055785890255</v>
       </c>
-      <c r="AI38" s="5">
-        <v>412.66111822426319</v>
+      <c r="AI38">
+        <v>495.19334186911584</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
@@ -5379,8 +5379,8 @@
       <c r="AH39" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI39" s="5">
-        <v>414.8527838024828</v>
+      <c r="AI39">
+        <v>497.82334056297935</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
@@ -5486,8 +5486,8 @@
       <c r="AH40" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI40" s="5">
-        <v>414.8527838024828</v>
+      <c r="AI40">
+        <v>497.82334056297935</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
@@ -5593,8 +5593,8 @@
       <c r="AH41" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI41" s="5">
-        <v>414.8527838024828</v>
+      <c r="AI41">
+        <v>497.82334056297935</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
@@ -5700,8 +5700,8 @@
       <c r="AH42" s="5">
         <v>12.47416684911069</v>
       </c>
-      <c r="AI42" s="5">
-        <v>426.56389491156574</v>
+      <c r="AI42">
+        <v>511.87667389387883</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
@@ -5807,8 +5807,8 @@
       <c r="AH43" s="5">
         <v>10.801666868146922</v>
       </c>
-      <c r="AI43" s="5">
-        <v>425.63334173108967</v>
+      <c r="AI43">
+        <v>510.76001007730764</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
@@ -5914,8 +5914,8 @@
       <c r="AH44" s="5">
         <v>14.008333571544952</v>
       </c>
-      <c r="AI44" s="5">
-        <v>458.97223125956953</v>
+      <c r="AI44">
+        <v>550.76667751148341</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
@@ -6021,8 +6021,8 @@
       <c r="AH45" s="5">
         <v>7.1547223484764499</v>
       </c>
-      <c r="AI45" s="5">
-        <v>324.48611763285265</v>
+      <c r="AI45">
+        <v>389.3833411594232</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.25">
@@ -6128,8 +6128,8 @@
       <c r="AH46" s="5">
         <v>6.6944445381975832</v>
       </c>
-      <c r="AI46" s="5">
-        <v>287.17778201711673</v>
+      <c r="AI46">
+        <v>344.61333842054012</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
@@ -6235,8 +6235,8 @@
       <c r="AH47" s="5">
         <v>4.4341667553409936</v>
       </c>
-      <c r="AI47" s="5">
-        <v>429.1027846506073</v>
+      <c r="AI47">
+        <v>514.92334158072867</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.25">
@@ -6342,8 +6342,8 @@
       <c r="AH48" s="5">
         <v>4.5591666952189476</v>
       </c>
-      <c r="AI48" s="5">
-        <v>352.47222829092709</v>
+      <c r="AI48">
+        <v>422.96667394911248</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.25">
@@ -6449,8 +6449,8 @@
       <c r="AH49" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI49" s="5">
-        <v>585.15834353077742</v>
+      <c r="AI49">
+        <v>702.19001223693294</v>
       </c>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.25">
@@ -6556,8 +6556,8 @@
       <c r="AH50" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI50" s="5">
-        <v>558.05000846460462</v>
+      <c r="AI50">
+        <v>669.66001015752556</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.25">
@@ -6663,8 +6663,8 @@
       <c r="AH51" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI51" s="5">
-        <v>558.05000846460462</v>
+      <c r="AI51">
+        <v>669.66001015752556</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.25">
@@ -6770,8 +6770,8 @@
       <c r="AH52" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI52" s="5">
-        <v>558.05000846460462</v>
+      <c r="AI52">
+        <v>669.66001015752556</v>
       </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
@@ -6877,8 +6877,8 @@
       <c r="AH53" s="5">
         <v>11.009722441848782</v>
       </c>
-      <c r="AI53" s="5">
-        <v>524.06667595584361</v>
+      <c r="AI53">
+        <v>628.88001114701228</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
@@ -6984,8 +6984,8 @@
       <c r="AH54" s="5">
         <v>9.6700001836236975</v>
       </c>
-      <c r="AI54" s="5">
-        <v>552.39167516099076</v>
+      <c r="AI54">
+        <v>662.87001019318893</v>
       </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.25">
@@ -7091,8 +7091,8 @@
       <c r="AH55" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI55" s="5">
-        <v>585.15834353077742</v>
+      <c r="AI55">
+        <v>702.19001223693294</v>
       </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.25">
@@ -7198,8 +7198,8 @@
       <c r="AH56" s="5">
         <v>7.8900001508080297</v>
       </c>
-      <c r="AI56" s="5">
-        <v>538.77223119036194</v>
+      <c r="AI56">
+        <v>646.52667742843425</v>
       </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.25">
@@ -7305,8 +7305,8 @@
       <c r="AH57" s="5">
         <v>5.0902778515799181</v>
       </c>
-      <c r="AI57" s="5">
-        <v>363.45278419926763</v>
+      <c r="AI57">
+        <v>436.14334103912114</v>
       </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
@@ -7412,8 +7412,8 @@
       <c r="AH58" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI58" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI58">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.25">
@@ -7519,8 +7519,8 @@
       <c r="AH59" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI59" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI59">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.25">
@@ -7626,8 +7626,8 @@
       <c r="AH60" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI60" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI60">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.25">
@@ -7733,8 +7733,8 @@
       <c r="AH61" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI61" s="5">
-        <v>573.27501039248375</v>
+      <c r="AI61">
+        <v>687.9300124709805</v>
       </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
@@ -7840,8 +7840,8 @@
       <c r="AH62" s="5">
         <v>12.402500250997642</v>
       </c>
-      <c r="AI62" s="5">
-        <v>547.28889729579282</v>
+      <c r="AI62">
+        <v>656.74667675495152</v>
       </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.25">
@@ -7947,8 +7947,8 @@
       <c r="AH63" s="5">
         <v>13.197500290266342</v>
       </c>
-      <c r="AI63" s="5">
-        <v>546.76667534187436</v>
+      <c r="AI63">
+        <v>656.12001041024928</v>
       </c>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.25">
@@ -8054,8 +8054,8 @@
       <c r="AH64" s="5">
         <v>14.578889134505557</v>
       </c>
-      <c r="AI64" s="5">
-        <v>652.91112009332414</v>
+      <c r="AI64">
+        <v>783.4933441119889</v>
       </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.25">
@@ -8161,8 +8161,8 @@
       <c r="AH65" s="5">
         <v>11.883889088572728</v>
       </c>
-      <c r="AI65" s="5">
-        <v>569.71112134224836</v>
+      <c r="AI65">
+        <v>683.65334561069801</v>
       </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.25">
@@ -8268,8 +8268,8 @@
       <c r="AH66" s="5">
         <v>12.213611334106988</v>
       </c>
-      <c r="AI66" s="5">
-        <v>525.42500915875041</v>
+      <c r="AI66">
+        <v>630.5100109905004</v>
       </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.25">
@@ -8375,8 +8375,8 @@
       <c r="AH67" s="5">
         <v>13.395278038394947</v>
       </c>
-      <c r="AI67" s="5">
-        <v>537.2777869978712</v>
+      <c r="AI67">
+        <v>644.73334439744553</v>
       </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.25">
@@ -8482,8 +8482,8 @@
       <c r="AH68" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI68" s="5">
-        <v>566.45556488446891</v>
+      <c r="AI68">
+        <v>679.74667786136274</v>
       </c>
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.25">
@@ -8589,8 +8589,8 @@
       <c r="AH69" s="5">
         <v>14.514166940645211</v>
       </c>
-      <c r="AI69" s="5">
-        <v>596.19445407142246</v>
+      <c r="AI69">
+        <v>715.4333448857069</v>
       </c>
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.25">
@@ -8696,8 +8696,8 @@
       <c r="AH70" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI70" s="5">
-        <v>566.45556488446891</v>
+      <c r="AI70">
+        <v>679.74667786136274</v>
       </c>
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.25">
@@ -8803,8 +8803,8 @@
       <c r="AH71" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI71" s="5">
-        <v>566.45556488446891</v>
+      <c r="AI71">
+        <v>679.74667786136274</v>
       </c>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.25">
@@ -8910,8 +8910,8 @@
       <c r="AH72" s="5">
         <v>13.200278020401795</v>
       </c>
-      <c r="AI72" s="5">
-        <v>570.10278523775446</v>
+      <c r="AI72">
+        <v>684.12334228530528</v>
       </c>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.25">
@@ -9017,8 +9017,8 @@
       <c r="AH73" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI73" s="5">
-        <v>620.17500988518202</v>
+      <c r="AI73">
+        <v>744.21001186221838</v>
       </c>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.25">
@@ -9124,8 +9124,8 @@
       <c r="AH74" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI74" s="5">
-        <v>620.17500988518202</v>
+      <c r="AI74">
+        <v>744.21001186221838</v>
       </c>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.25">
@@ -9231,8 +9231,8 @@
       <c r="AH75" s="5">
         <v>12.714166869243813</v>
       </c>
-      <c r="AI75" s="5">
-        <v>603.38612122357722</v>
+      <c r="AI75">
+        <v>724.0633454682926</v>
       </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.25">
@@ -9338,8 +9338,8 @@
       <c r="AH76" s="5">
         <v>14.380278021987113</v>
       </c>
-      <c r="AI76" s="5">
-        <v>491.92778695105682</v>
+      <c r="AI76">
+        <v>590.31334434126813</v>
       </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.25">
@@ -9445,8 +9445,8 @@
       <c r="AH77" s="5">
         <v>15.016111336586375</v>
       </c>
-      <c r="AI77" s="5">
-        <v>523.51389659030576</v>
+      <c r="AI77">
+        <v>628.21667590836682</v>
       </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.25">
@@ -9552,8 +9552,8 @@
       <c r="AH78" s="5">
         <v>14.131666897899574</v>
       </c>
-      <c r="AI78" s="5">
-        <v>609.11667874124316</v>
+      <c r="AI78">
+        <v>730.94001448949177</v>
       </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.25">
@@ -9659,8 +9659,8 @@
       <c r="AH79" s="5">
         <v>14.880833575605518</v>
       </c>
-      <c r="AI79" s="5">
-        <v>559.15000913561221</v>
+      <c r="AI79">
+        <v>670.98001096273458</v>
       </c>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.25">
@@ -9766,8 +9766,8 @@
       <c r="AH80" s="5">
         <v>16.243055798009866</v>
       </c>
-      <c r="AI80" s="5">
-        <v>974.54724013743305</v>
+      <c r="AI80">
+        <v>1169.4566881649196</v>
       </c>
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.25">
@@ -9873,8 +9873,8 @@
       <c r="AH81" s="5">
         <v>16.389166925619875</v>
       </c>
-      <c r="AI81" s="5">
-        <v>1045.9916839278819</v>
+      <c r="AI81">
+        <v>1255.1900207134584</v>
       </c>
     </row>
     <row r="82" spans="1:35" x14ac:dyDescent="0.25">
@@ -9980,8 +9980,8 @@
       <c r="AH82" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI82" s="5">
-        <v>972.81945985162429</v>
+      <c r="AI82">
+        <v>1167.3833518219492</v>
       </c>
     </row>
     <row r="83" spans="1:35" x14ac:dyDescent="0.25">
@@ -10087,8 +10087,8 @@
       <c r="AH83" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI83" s="5">
-        <v>972.81945985162429</v>
+      <c r="AI83">
+        <v>1167.3833518219492</v>
       </c>
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.25">
@@ -10194,8 +10194,8 @@
       <c r="AH84" s="5">
         <v>15.054166897386313</v>
       </c>
-      <c r="AI84" s="5">
-        <v>680.59445726954277</v>
+      <c r="AI84">
+        <v>816.7133487234513</v>
       </c>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.25">
@@ -10301,8 +10301,8 @@
       <c r="AH85" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI85" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI85">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.25">
@@ -10408,8 +10408,8 @@
       <c r="AH86" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI86" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI86">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.25">
@@ -10515,8 +10515,8 @@
       <c r="AH87" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI87" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI87">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.25">
@@ -10622,8 +10622,8 @@
       <c r="AH88" s="5">
         <v>16.396111346284549</v>
       </c>
-      <c r="AI88" s="5">
-        <v>1023.2333520479086</v>
+      <c r="AI88">
+        <v>1227.8800224574904</v>
       </c>
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.25">
@@ -10729,8 +10729,8 @@
       <c r="AH89" s="5">
         <v>15.944722454353339</v>
       </c>
-      <c r="AI89" s="5">
-        <v>973.28057178854942</v>
+      <c r="AI89">
+        <v>1167.9366861462593</v>
       </c>
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.25">
@@ -10836,8 +10836,8 @@
       <c r="AH90" s="5">
         <v>15.40638912299441</v>
       </c>
-      <c r="AI90" s="5">
-        <v>937.34723641309472</v>
+      <c r="AI90">
+        <v>1124.8166836957137</v>
       </c>
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.25">
@@ -10943,8 +10943,8 @@
       <c r="AH91" s="5">
         <v>14.980833584670391</v>
       </c>
-      <c r="AI91" s="5">
-        <v>755.10834456897442</v>
+      <c r="AI91">
+        <v>906.1300134827693</v>
       </c>
     </row>
     <row r="92" spans="1:35" x14ac:dyDescent="0.25">
@@ -11050,8 +11050,8 @@
       <c r="AH92" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI92" s="5">
-        <v>916.66668113569415</v>
+      <c r="AI92">
+        <v>1100.000017362833</v>
       </c>
     </row>
     <row r="93" spans="1:35" x14ac:dyDescent="0.25">
@@ -11157,8 +11157,8 @@
       <c r="AH93" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI93" s="5">
-        <v>916.66668113569415</v>
+      <c r="AI93">
+        <v>1100.000017362833</v>
       </c>
     </row>
     <row r="94" spans="1:35" x14ac:dyDescent="0.25">
@@ -11264,8 +11264,8 @@
       <c r="AH94" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI94" s="5">
-        <v>976.1416809668558</v>
+      <c r="AI94">
+        <v>1171.370017160227</v>
       </c>
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.25">
@@ -11371,8 +11371,8 @@
       <c r="AH95" s="5">
         <v>15.691944675313103</v>
       </c>
-      <c r="AI95" s="5">
-        <v>918.32779509491388</v>
+      <c r="AI95">
+        <v>1101.9933541138967</v>
       </c>
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.25">
@@ -11478,8 +11478,8 @@
       <c r="AH96" s="5">
         <v>15.582500197138224</v>
       </c>
-      <c r="AI96" s="5">
-        <v>711.19723644293845</v>
+      <c r="AI96">
+        <v>853.43668373152616</v>
       </c>
     </row>
     <row r="97" spans="1:35" x14ac:dyDescent="0.25">
@@ -11585,8 +11585,8 @@
       <c r="AH97" s="5">
         <v>16.058055824786425</v>
       </c>
-      <c r="AI97" s="5">
-        <v>808.70001078314249</v>
+      <c r="AI97">
+        <v>970.44001293977101</v>
       </c>
     </row>
     <row r="98" spans="1:35" x14ac:dyDescent="0.25">
@@ -11692,8 +11692,8 @@
       <c r="AH98" s="5">
         <v>15.946111321780418</v>
       </c>
-      <c r="AI98" s="5">
-        <v>830.38057103566825</v>
+      <c r="AI98">
+        <v>996.45668524280188</v>
       </c>
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.25">
@@ -11799,8 +11799,8 @@
       <c r="AH99" s="5">
         <v>16.454722446203231</v>
       </c>
-      <c r="AI99" s="5">
-        <v>965.53890664647849</v>
+      <c r="AI99">
+        <v>1158.6466879757743</v>
       </c>
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.25">
@@ -11906,8 +11906,8 @@
       <c r="AH100" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI100" s="5">
-        <v>1177.1250198669732</v>
+      <c r="AI100">
+        <v>1412.5500238403679</v>
       </c>
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.25">
@@ -12013,8 +12013,8 @@
       <c r="AH101" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI101" s="5">
-        <v>1177.1250198669732</v>
+      <c r="AI101">
+        <v>1412.5500238403679</v>
       </c>
     </row>
     <row r="102" spans="1:35" x14ac:dyDescent="0.25">
@@ -12120,8 +12120,8 @@
       <c r="AH102" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI102" s="5">
-        <v>1177.1250198669732</v>
+      <c r="AI102">
+        <v>1412.5500238403679</v>
       </c>
     </row>
     <row r="103" spans="1:35" x14ac:dyDescent="0.25">
@@ -12227,8 +12227,8 @@
       <c r="AH103" s="5">
         <v>15.962500282625358</v>
       </c>
-      <c r="AI103" s="5">
-        <v>1251.4500212321677</v>
+      <c r="AI103">
+        <v>1501.7400254786014</v>
       </c>
     </row>
     <row r="104" spans="1:35" x14ac:dyDescent="0.25">
@@ -12334,8 +12334,8 @@
       <c r="AH104" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI104" s="5">
-        <v>1191.1305749962728</v>
+      <c r="AI104">
+        <v>1429.3566899955272</v>
       </c>
     </row>
     <row r="105" spans="1:35" x14ac:dyDescent="0.25">
@@ -12441,8 +12441,8 @@
       <c r="AH105" s="5">
         <v>17.36972248951594</v>
       </c>
-      <c r="AI105" s="5">
-        <v>1349.7722442580593</v>
+      <c r="AI105">
+        <v>1619.7266931096713</v>
       </c>
     </row>
     <row r="106" spans="1:35" x14ac:dyDescent="0.25">
@@ -12548,8 +12548,8 @@
       <c r="AH106" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI106" s="5">
-        <v>1191.1305749962728</v>
+      <c r="AI106">
+        <v>1429.3566899955272</v>
       </c>
     </row>
     <row r="107" spans="1:35" x14ac:dyDescent="0.25">
@@ -12655,8 +12655,8 @@
       <c r="AH107" s="5">
         <v>16.991666977935367</v>
       </c>
-      <c r="AI107" s="5">
-        <v>1217.8805788490508</v>
+      <c r="AI107">
+        <v>1461.4566946188609</v>
       </c>
     </row>
     <row r="108" spans="1:35" x14ac:dyDescent="0.25">
@@ -12762,8 +12762,8 @@
       <c r="AH108" s="5">
         <v>17.177500254909198</v>
       </c>
-      <c r="AI108" s="5">
-        <v>1147.3750202815152</v>
+      <c r="AI108">
+        <v>1376.8500243378182</v>
       </c>
     </row>
     <row r="109" spans="1:35" x14ac:dyDescent="0.25">
@@ -12869,8 +12869,8 @@
       <c r="AH109" s="5">
         <v>16.59805584020085</v>
       </c>
-      <c r="AI109" s="5">
-        <v>1339.4305793709225</v>
+      <c r="AI109">
+        <v>1607.316695245107</v>
       </c>
     </row>
     <row r="110" spans="1:35" x14ac:dyDescent="0.25">
@@ -12976,8 +12976,8 @@
       <c r="AH110" s="5">
         <v>18.400555811987982</v>
       </c>
-      <c r="AI110" s="5">
-        <v>1391.8944691154693</v>
+      <c r="AI110">
+        <v>1670.273362938563</v>
       </c>
     </row>
     <row r="111" spans="1:35" x14ac:dyDescent="0.25">
@@ -13083,8 +13083,8 @@
       <c r="AH111" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI111" s="5">
-        <v>1104.4277913001263</v>
+      <c r="AI111">
+        <v>1325.3133495601514</v>
       </c>
     </row>
     <row r="112" spans="1:35" x14ac:dyDescent="0.25">
@@ -13190,8 +13190,8 @@
       <c r="AH112" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI112" s="5">
-        <v>1104.4277913001263</v>
+      <c r="AI112">
+        <v>1325.3133495601514</v>
       </c>
     </row>
     <row r="113" spans="1:35" x14ac:dyDescent="0.25">
@@ -13297,8 +13297,8 @@
       <c r="AH113" s="5">
         <v>16.237500274015797</v>
       </c>
-      <c r="AI113" s="5">
-        <v>1115.8777972248693</v>
+      <c r="AI113">
+        <v>1339.0533566698432</v>
       </c>
     </row>
     <row r="114" spans="1:35" x14ac:dyDescent="0.25">
@@ -13404,8 +13404,8 @@
       <c r="AH114" s="5">
         <v>16.611111394564311</v>
       </c>
-      <c r="AI114" s="5">
-        <v>1209.9305740810103</v>
+      <c r="AI114">
+        <v>1451.9166888972125</v>
       </c>
     </row>
     <row r="115" spans="1:35" x14ac:dyDescent="0.25">
@@ -13511,8 +13511,8 @@
       <c r="AH115" s="5">
         <v>16.962222494681676</v>
       </c>
-      <c r="AI115" s="5">
-        <v>1292.7444617682033</v>
+      <c r="AI115">
+        <v>1551.293354121844</v>
       </c>
     </row>
     <row r="116" spans="1:35" x14ac:dyDescent="0.25">
@@ -13618,8 +13618,8 @@
       <c r="AH116" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI116" s="5">
-        <v>1253.5278008513981</v>
+      <c r="AI116">
+        <v>1504.2333610216776</v>
       </c>
     </row>
     <row r="117" spans="1:35" x14ac:dyDescent="0.25">
@@ -13725,8 +13725,8 @@
       <c r="AH117" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI117" s="5">
-        <v>1253.5278008513981</v>
+      <c r="AI117">
+        <v>1504.2333610216776</v>
       </c>
     </row>
     <row r="118" spans="1:35" x14ac:dyDescent="0.25">
@@ -13832,8 +13832,8 @@
       <c r="AH118" s="5">
         <v>17.300555813312531</v>
       </c>
-      <c r="AI118" s="5">
-        <v>1423.0694724387592</v>
+      <c r="AI118">
+        <v>1707.6833669265111</v>
       </c>
     </row>
     <row r="119" spans="1:35" x14ac:dyDescent="0.25">
@@ -13939,8 +13939,8 @@
       <c r="AH119" s="5">
         <v>16.892500269412995</v>
       </c>
-      <c r="AI119" s="5">
-        <v>1336.4194651179844</v>
+      <c r="AI119">
+        <v>1603.7033581415812</v>
       </c>
     </row>
     <row r="120" spans="1:35" x14ac:dyDescent="0.25">
@@ -14046,8 +14046,8 @@
       <c r="AH120" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI120" s="5">
-        <v>1283.6750270724297</v>
+      <c r="AI120">
+        <v>1540.4100324869155</v>
       </c>
     </row>
     <row r="121" spans="1:35" x14ac:dyDescent="0.25">
@@ -14153,8 +14153,8 @@
       <c r="AH121" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI121" s="5">
-        <v>1283.6750270724297</v>
+      <c r="AI121">
+        <v>1540.4100324869155</v>
       </c>
     </row>
     <row r="122" spans="1:35" x14ac:dyDescent="0.25">
@@ -14260,8 +14260,8 @@
       <c r="AH122" s="5">
         <v>17.377222496933406</v>
       </c>
-      <c r="AI122" s="5">
-        <v>1343.3778014977772</v>
+      <c r="AI122">
+        <v>1612.0533617973329</v>
       </c>
     </row>
     <row r="123" spans="1:35" x14ac:dyDescent="0.25">
@@ -14367,8 +14367,8 @@
       <c r="AH123" s="5">
         <v>18.61972255706787</v>
       </c>
-      <c r="AI123" s="5">
-        <v>1319.411135070854</v>
+      <c r="AI123">
+        <v>1583.2933620850245</v>
       </c>
     </row>
     <row r="124" spans="1:35" x14ac:dyDescent="0.25">
@@ -14474,8 +14474,8 @@
       <c r="AH124" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI124" s="5">
-        <v>1485.5694680930012</v>
+      <c r="AI124">
+        <v>1782.6833617116015</v>
       </c>
     </row>
     <row r="125" spans="1:35" x14ac:dyDescent="0.25">
@@ -14581,8 +14581,8 @@
       <c r="AH125" s="5">
         <v>21.330278105205959</v>
       </c>
-      <c r="AI125" s="5">
-        <v>1181.3278022805848</v>
+      <c r="AI125">
+        <v>1417.5933627367019</v>
       </c>
     </row>
     <row r="126" spans="1:35" x14ac:dyDescent="0.25">
@@ -14688,8 +14688,8 @@
       <c r="AH126" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI126" s="5">
-        <v>1485.5694680930012</v>
+      <c r="AI126">
+        <v>1782.6833617116015</v>
       </c>
     </row>
     <row r="127" spans="1:35" x14ac:dyDescent="0.25">
@@ -14795,8 +14795,8 @@
       <c r="AH127" s="5">
         <v>14.705277992950545</v>
       </c>
-      <c r="AI127" s="5">
-        <v>545.45556631498039</v>
+      <c r="AI127">
+        <v>654.54667957797642</v>
       </c>
     </row>
     <row r="128" spans="1:35" x14ac:dyDescent="0.25">
@@ -14902,8 +14902,8 @@
       <c r="AH128" s="5">
         <v>15.146666885043183</v>
       </c>
-      <c r="AI128" s="5">
-        <v>511.14445323290101</v>
+      <c r="AI128">
+        <v>613.37334387948113</v>
       </c>
     </row>
     <row r="129" spans="1:35" x14ac:dyDescent="0.25">
@@ -15009,8 +15009,8 @@
       <c r="AH129" s="5">
         <v>15.114166894327436</v>
       </c>
-      <c r="AI129" s="5">
-        <v>552.70001020903385</v>
+      <c r="AI129">
+        <v>663.24001225084066</v>
       </c>
     </row>
     <row r="130" spans="1:35" x14ac:dyDescent="0.25">
@@ -15116,8 +15116,8 @@
       <c r="AH130" s="5">
         <v>14.685000222010745</v>
       </c>
-      <c r="AI130" s="5">
-        <v>516.12222921537852</v>
+      <c r="AI130">
+        <v>619.34667505845425</v>
       </c>
     </row>
     <row r="131" spans="1:35" x14ac:dyDescent="0.25">
@@ -15223,8 +15223,8 @@
       <c r="AH131" s="5">
         <v>14.560555819484096</v>
       </c>
-      <c r="AI131" s="5">
-        <v>486.50834265165031</v>
+      <c r="AI131">
+        <v>583.81001118198037</v>
       </c>
     </row>
     <row r="132" spans="1:35" x14ac:dyDescent="0.25">
@@ -15330,8 +15330,8 @@
       <c r="AH132" s="5">
         <v>14.925000269276401</v>
       </c>
-      <c r="AI132" s="5">
-        <v>587.93612111028699</v>
+      <c r="AI132">
+        <v>705.52334533234432</v>
       </c>
     </row>
     <row r="133" spans="1:35" x14ac:dyDescent="0.25">
@@ -15437,8 +15437,8 @@
       <c r="AH133" s="5">
         <v>14.240833549056616</v>
       </c>
-      <c r="AI133" s="5">
-        <v>578.55278752330275</v>
+      <c r="AI133">
+        <v>694.26334502796328</v>
       </c>
     </row>
     <row r="134" spans="1:35" x14ac:dyDescent="0.25">
@@ -15544,8 +15544,8 @@
       <c r="AH134" s="5">
         <v>15.481111367895371</v>
       </c>
-      <c r="AI134" s="5">
-        <v>664.15001225223148</v>
+      <c r="AI134">
+        <v>796.98001470267775</v>
       </c>
     </row>
     <row r="135" spans="1:35" x14ac:dyDescent="0.25">
@@ -15651,8 +15651,8 @@
       <c r="AH135" s="5">
         <v>15.808611411021815</v>
       </c>
-      <c r="AI135" s="5">
-        <v>732.42223528027534</v>
+      <c r="AI135">
+        <v>878.90668233633039</v>
       </c>
     </row>
     <row r="136" spans="1:35" x14ac:dyDescent="0.25">
@@ -15758,8 +15758,8 @@
       <c r="AH136" s="5">
         <v>16.348055789868038</v>
       </c>
-      <c r="AI136" s="5">
-        <v>706.5083447649248</v>
+      <c r="AI136">
+        <v>847.81001371790967</v>
       </c>
     </row>
     <row r="137" spans="1:35" x14ac:dyDescent="0.25">
@@ -15865,8 +15865,8 @@
       <c r="AH137" s="5">
         <v>13.885278014466166</v>
       </c>
-      <c r="AI137" s="5">
-        <v>482.41945241867666</v>
+      <c r="AI137">
+        <v>578.90334290241196</v>
       </c>
     </row>
     <row r="138" spans="1:35" x14ac:dyDescent="0.25">
@@ -15972,8 +15972,8 @@
       <c r="AH138" s="5">
         <v>17.218055825101004</v>
       </c>
-      <c r="AI138" s="5">
-        <v>1039.4416841963928</v>
+      <c r="AI138">
+        <v>1247.3300210356713</v>
       </c>
     </row>
     <row r="139" spans="1:35" x14ac:dyDescent="0.25">
@@ -16079,8 +16079,8 @@
       <c r="AH139" s="5">
         <v>17.671944708956612</v>
       </c>
-      <c r="AI139" s="5">
-        <v>1200.402797886067</v>
+      <c r="AI139">
+        <v>1440.4833574632803</v>
       </c>
     </row>
     <row r="140" spans="1:35" x14ac:dyDescent="0.25">
@@ -16186,8 +16186,8 @@
       <c r="AH140" s="5">
         <v>17.840000283055836</v>
       </c>
-      <c r="AI140" s="5">
-        <v>1233.1194645899038</v>
+      <c r="AI140">
+        <v>1479.7433575078844</v>
       </c>
     </row>
     <row r="141" spans="1:35" x14ac:dyDescent="0.25">
@@ -16293,8 +16293,8 @@
       <c r="AH141" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI141" s="5">
-        <v>1830.8222555894818</v>
+      <c r="AI141">
+        <v>2196.9867067073783</v>
       </c>
     </row>
     <row r="142" spans="1:35" x14ac:dyDescent="0.25">
@@ -16400,8 +16400,8 @@
       <c r="AH142" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI142" s="5">
-        <v>1830.8222555894818</v>
+      <c r="AI142">
+        <v>2196.9867067073783</v>
       </c>
     </row>
     <row r="143" spans="1:35" x14ac:dyDescent="0.25">
@@ -16507,8 +16507,8 @@
       <c r="AH143" s="5">
         <v>22.497500356038412</v>
       </c>
-      <c r="AI143" s="5">
-        <v>1457.10002325558</v>
+      <c r="AI143">
+        <v>1748.520027906696</v>
       </c>
     </row>
     <row r="144" spans="1:35" x14ac:dyDescent="0.25">
@@ -16614,8 +16614,8 @@
       <c r="AH144" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI144" s="5">
-        <v>834.33056925133701</v>
+      <c r="AI144">
+        <v>1001.1966831016044</v>
       </c>
     </row>
     <row r="145" spans="1:35" x14ac:dyDescent="0.25">
@@ -16721,8 +16721,8 @@
       <c r="AH145" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI145" s="5">
-        <v>834.33056925133701</v>
+      <c r="AI145">
+        <v>1001.1966831016044</v>
       </c>
     </row>
     <row r="146" spans="1:35" x14ac:dyDescent="0.25">
@@ -16828,8 +16828,8 @@
       <c r="AH146" s="5">
         <v>16.466389189826117</v>
       </c>
-      <c r="AI146" s="5">
-        <v>841.05279137276943</v>
+      <c r="AI146">
+        <v>1009.2633496473233</v>
       </c>
     </row>
     <row r="147" spans="1:35" x14ac:dyDescent="0.25">
@@ -16935,8 +16935,8 @@
       <c r="AH147" s="5">
         <v>18.550555888811747</v>
       </c>
-      <c r="AI147" s="5">
-        <v>921.3805729982754</v>
+      <c r="AI147">
+        <v>1105.6566875979304</v>
       </c>
     </row>
     <row r="148" spans="1:35" x14ac:dyDescent="0.25">
@@ -17042,8 +17042,8 @@
       <c r="AH148" s="5">
         <v>16.811666933695474</v>
       </c>
-      <c r="AI148" s="5">
-        <v>773.31945808397393</v>
+      <c r="AI148">
+        <v>927.98334970076883</v>
       </c>
     </row>
     <row r="149" spans="1:35" x14ac:dyDescent="0.25">
@@ -17149,8 +17149,8 @@
       <c r="AH149" s="5">
         <v>16.939166976345909</v>
       </c>
-      <c r="AI149" s="5">
-        <v>819.41945890420016</v>
+      <c r="AI149">
+        <v>983.30335068504019</v>
       </c>
     </row>
     <row r="150" spans="1:35" x14ac:dyDescent="0.25">
@@ -17256,8 +17256,8 @@
       <c r="AH150" s="5">
         <v>17.050555853048959</v>
       </c>
-      <c r="AI150" s="5">
-        <v>892.72501441505233</v>
+      <c r="AI150">
+        <v>1071.2700172980626</v>
       </c>
     </row>
     <row r="151" spans="1:35" x14ac:dyDescent="0.25">
@@ -17363,8 +17363,8 @@
       <c r="AH151" s="5">
         <v>18.485833643542396</v>
       </c>
-      <c r="AI151" s="5">
-        <v>872.06945833232669</v>
+      <c r="AI151">
+        <v>1046.4833499987919</v>
       </c>
     </row>
     <row r="152" spans="1:35" x14ac:dyDescent="0.25">
@@ -17470,8 +17470,8 @@
       <c r="AH152" s="5">
         <v>17.482500301467049</v>
       </c>
-      <c r="AI152" s="5">
-        <v>860.67501521627935</v>
+      <c r="AI152">
+        <v>1032.8100182595351</v>
       </c>
     </row>
     <row r="153" spans="1:35" x14ac:dyDescent="0.25">
@@ -17577,8 +17577,8 @@
       <c r="AH153" s="5">
         <v>17.544166929192013</v>
       </c>
-      <c r="AI153" s="5">
-        <v>887.32223747173953</v>
+      <c r="AI153">
+        <v>1064.7866849660873</v>
       </c>
     </row>
     <row r="154" spans="1:35" x14ac:dyDescent="0.25">
@@ -17684,8 +17684,8 @@
       <c r="AH154" s="5">
         <v>17.002222526735729</v>
       </c>
-      <c r="AI154" s="5">
-        <v>907.56946346494885</v>
+      <c r="AI154">
+        <v>1089.0833561579386</v>
       </c>
     </row>
     <row r="155" spans="1:35" x14ac:dyDescent="0.25">
@@ -17791,8 +17791,8 @@
       <c r="AH155" s="5">
         <v>16.162500272856818</v>
       </c>
-      <c r="AI155" s="5">
-        <v>937.16668129629556</v>
+      <c r="AI155">
+        <v>1124.6000175555548</v>
       </c>
     </row>
     <row r="156" spans="1:35" x14ac:dyDescent="0.25">
@@ -17898,8 +17898,8 @@
       <c r="AH156" s="5">
         <v>13.510278080569373</v>
       </c>
-      <c r="AI156" s="5">
-        <v>787.63334739849802</v>
+      <c r="AI156">
+        <v>945.16001687819755</v>
       </c>
     </row>
     <row r="157" spans="1:35" x14ac:dyDescent="0.25">
@@ -18005,8 +18005,8 @@
       <c r="AH157" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI157" s="5">
-        <v>549.71389919084811</v>
+      <c r="AI157">
+        <v>659.65667902901771</v>
       </c>
     </row>
     <row r="158" spans="1:35" x14ac:dyDescent="0.25">
@@ -18112,8 +18112,8 @@
       <c r="AH158" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI158" s="5">
-        <v>549.71389919084811</v>
+      <c r="AI158">
+        <v>659.65667902901771</v>
       </c>
     </row>
     <row r="159" spans="1:35" x14ac:dyDescent="0.25">
@@ -18219,8 +18219,8 @@
       <c r="AH159" s="5">
         <v>11.430000214464963</v>
       </c>
-      <c r="AI159" s="5">
-        <v>464.2444530808263</v>
+      <c r="AI159">
+        <v>557.09334369699161</v>
       </c>
     </row>
     <row r="160" spans="1:35" x14ac:dyDescent="0.25">
@@ -18326,8 +18326,8 @@
       <c r="AH160" s="5">
         <v>7.7977779119999875</v>
       </c>
-      <c r="AI160" s="5">
-        <v>304.89444963427053</v>
+      <c r="AI160">
+        <v>365.87333956112462</v>
       </c>
     </row>
     <row r="161" spans="1:35" x14ac:dyDescent="0.25">
@@ -18433,8 +18433,8 @@
       <c r="AH161" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI161" s="5">
-        <v>186.40278092482023</v>
+      <c r="AI161">
+        <v>223.68333710978428</v>
       </c>
     </row>
     <row r="162" spans="1:35" x14ac:dyDescent="0.25">
@@ -18540,8 +18540,8 @@
       <c r="AH162" s="5">
         <v>7.6125001351452539</v>
       </c>
-      <c r="AI162" s="5">
-        <v>318.32222728969322</v>
+      <c r="AI162">
+        <v>381.98667274763187</v>
       </c>
     </row>
     <row r="163" spans="1:35" x14ac:dyDescent="0.25">
@@ -18647,8 +18647,8 @@
       <c r="AH163" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI163" s="5">
-        <v>186.40278092482023</v>
+      <c r="AI163">
+        <v>223.68333710978428</v>
       </c>
     </row>
     <row r="164" spans="1:35" x14ac:dyDescent="0.25">
@@ -18754,8 +18754,8 @@
       <c r="AH164" s="5">
         <v>5.8491667841457655</v>
       </c>
-      <c r="AI164" s="5">
-        <v>183.68611463511155</v>
+      <c r="AI164">
+        <v>220.42333756213387</v>
       </c>
     </row>
     <row r="165" spans="1:35" x14ac:dyDescent="0.25">
@@ -18861,8 +18861,8 @@
       <c r="AH165" s="5">
         <v>4.4586112032747929</v>
       </c>
-      <c r="AI165" s="5">
-        <v>193.72222591543363</v>
+      <c r="AI165">
+        <v>232.46667109852035</v>
       </c>
     </row>
     <row r="166" spans="1:35" x14ac:dyDescent="0.25">
@@ -18968,8 +18968,8 @@
       <c r="AH166" s="5">
         <v>5.5380556673639347</v>
       </c>
-      <c r="AI166" s="5">
-        <v>173.45555842088328</v>
+      <c r="AI166">
+        <v>208.14667010505994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mean values of the climate variables. Also add the inverse distance weighting method.
</commit_message>
<xml_diff>
--- a/with climate data and WWTP coordinate.xlsx
+++ b/with climate data and WWTP coordinate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19245" yWindow="0" windowWidth="19155" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="19245" yWindow="0" windowWidth="9555" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bundled" sheetId="1" r:id="rId1"/>
@@ -956,13 +956,13 @@
     <t>Latitude</t>
   </si>
   <si>
-    <t>Longtitude</t>
-  </si>
-  <si>
     <t>mean annual temperature (celsius degree)</t>
   </si>
   <si>
     <t>mean annual precipitation (mm)</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1300,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ6" sqref="AJ6"/>
+      <selection pane="topRight" activeCell="AJ24" sqref="AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1315,7 @@
     <col min="32" max="32" width="11" style="2"/>
     <col min="33" max="33" width="46.625" style="2" customWidth="1"/>
     <col min="34" max="34" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.25" customWidth="1"/>
+    <col min="35" max="35" width="30.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -1413,16 +1413,16 @@
         <v>59</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AG1" s="2" t="s">
         <v>307</v>
       </c>
       <c r="AH1" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
       <c r="AH2" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="5">
         <v>482.52000884711742</v>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       <c r="AH3" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI3">
+      <c r="AI3" s="5">
         <v>482.52000884711742</v>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       <c r="AH4" s="5">
         <v>13.064444640423689</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="5">
         <v>482.52000884711742</v>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       <c r="AH5" s="5">
         <v>12.141944655051661</v>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="5">
         <v>467.22000859454272</v>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       <c r="AH6" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="5">
         <v>1264.0833567380905</v>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="AH7" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI7">
+      <c r="AI7" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       <c r="AH8" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI8">
+      <c r="AI8" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       <c r="AH9" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       <c r="AH10" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI10">
+      <c r="AI10" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2461,7 +2461,7 @@
       <c r="AH11" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI11">
+      <c r="AI11" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       <c r="AH12" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI12">
+      <c r="AI12" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       <c r="AH13" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI13">
+      <c r="AI13" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
       <c r="AH14" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI14">
+      <c r="AI14" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       <c r="AH15" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI15">
+      <c r="AI15" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       <c r="AH16" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI16">
+      <c r="AI16" s="5">
         <v>1306.2633549531301</v>
       </c>
     </row>
@@ -3085,7 +3085,7 @@
       <c r="AH17" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI17">
+      <c r="AI17" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       <c r="AH18" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI18">
+      <c r="AI18" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -3293,7 +3293,7 @@
       <c r="AH19" s="5">
         <v>16.841666924622324</v>
       </c>
-      <c r="AI19">
+      <c r="AI19" s="5">
         <v>1306.2633549531301</v>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       <c r="AH20" s="5">
         <v>16.642222461766668</v>
       </c>
-      <c r="AI20">
+      <c r="AI20" s="5">
         <v>1264.0833567380905</v>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       <c r="AH21" s="5">
         <v>16.460000312825045</v>
       </c>
-      <c r="AI21">
+      <c r="AI21" s="5">
         <v>1227.7666888475419</v>
       </c>
     </row>
@@ -3605,7 +3605,7 @@
       <c r="AH22" s="5">
         <v>13.163889099905889</v>
       </c>
-      <c r="AI22">
+      <c r="AI22" s="5">
         <v>489.91334197868906</v>
       </c>
     </row>
@@ -3709,7 +3709,7 @@
       <c r="AH23" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI23">
+      <c r="AI23" s="5">
         <v>1152.1833533684412</v>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       <c r="AH24" s="5">
         <v>17.651111385557385</v>
       </c>
-      <c r="AI24">
+      <c r="AI24" s="5">
         <v>1146.9466877460479</v>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
       <c r="AH25" s="5">
         <v>15.193055835366248</v>
       </c>
-      <c r="AI25">
+      <c r="AI25" s="5">
         <v>1171.4066875537237</v>
       </c>
     </row>
@@ -4021,7 +4021,7 @@
       <c r="AH26" s="5">
         <v>14.228333567414019</v>
       </c>
-      <c r="AI26">
+      <c r="AI26" s="5">
         <v>1074.7333531796933</v>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       <c r="AH27" s="5">
         <v>17.096944735447565</v>
       </c>
-      <c r="AI27">
+      <c r="AI27" s="5">
         <v>1152.1833533684412</v>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
       <c r="AH28" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI28">
+      <c r="AI28" s="5">
         <v>1096.6566830794015</v>
       </c>
     </row>
@@ -4333,7 +4333,7 @@
       <c r="AH29" s="5">
         <v>18.581111400657228</v>
       </c>
-      <c r="AI29">
+      <c r="AI29" s="5">
         <v>1096.6566830794015</v>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       <c r="AH30" s="5">
         <v>15.2763891518116</v>
       </c>
-      <c r="AI30">
+      <c r="AI30" s="5">
         <v>1093.6533483068149</v>
       </c>
     </row>
@@ -4541,7 +4541,7 @@
       <c r="AH31" s="5">
         <v>15.491389160023795</v>
       </c>
-      <c r="AI31">
+      <c r="AI31" s="5">
         <v>1143.6800213019053</v>
       </c>
     </row>
@@ -4645,7 +4645,7 @@
       <c r="AH32" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI32">
+      <c r="AI32" s="5">
         <v>1143.4166879415511</v>
       </c>
     </row>
@@ -4749,7 +4749,7 @@
       <c r="AH33" s="5">
         <v>16.513889181613923</v>
       </c>
-      <c r="AI33">
+      <c r="AI33" s="5">
         <v>1143.4166879415511</v>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       <c r="AH34" s="5">
         <v>14.283055821309487</v>
       </c>
-      <c r="AI34">
+      <c r="AI34" s="5">
         <v>1064.9600166936716</v>
       </c>
     </row>
@@ -4957,7 +4957,7 @@
       <c r="AH35" s="5">
         <v>16.284166936079661</v>
       </c>
-      <c r="AI35">
+      <c r="AI35" s="5">
         <v>1184.4866863250732</v>
       </c>
     </row>
@@ -5061,7 +5061,7 @@
       <c r="AH36" s="5">
         <v>18.087500296698675</v>
       </c>
-      <c r="AI36">
+      <c r="AI36" s="5">
         <v>1125.8433512528738</v>
       </c>
     </row>
@@ -5165,7 +5165,7 @@
       <c r="AH37" s="5">
         <v>14.717222467395995</v>
       </c>
-      <c r="AI37">
+      <c r="AI37" s="5">
         <v>1169.6400195121764</v>
       </c>
     </row>
@@ -5272,7 +5272,7 @@
       <c r="AH38" s="5">
         <v>13.463055785890255</v>
       </c>
-      <c r="AI38">
+      <c r="AI38" s="5">
         <v>495.19334186911584</v>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
       <c r="AH39" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI39">
+      <c r="AI39" s="5">
         <v>497.82334056297935</v>
       </c>
     </row>
@@ -5486,7 +5486,7 @@
       <c r="AH40" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI40">
+      <c r="AI40" s="5">
         <v>497.82334056297935</v>
       </c>
     </row>
@@ -5593,7 +5593,7 @@
       <c r="AH41" s="5">
         <v>12.048055728959541</v>
       </c>
-      <c r="AI41">
+      <c r="AI41" s="5">
         <v>497.82334056297935</v>
       </c>
     </row>
@@ -5700,7 +5700,7 @@
       <c r="AH42" s="5">
         <v>12.47416684911069</v>
       </c>
-      <c r="AI42">
+      <c r="AI42" s="5">
         <v>511.87667389387883</v>
       </c>
     </row>
@@ -5807,7 +5807,7 @@
       <c r="AH43" s="5">
         <v>10.801666868146922</v>
       </c>
-      <c r="AI43">
+      <c r="AI43" s="5">
         <v>510.76001007730764</v>
       </c>
     </row>
@@ -5914,7 +5914,7 @@
       <c r="AH44" s="5">
         <v>14.008333571544952</v>
       </c>
-      <c r="AI44">
+      <c r="AI44" s="5">
         <v>550.76667751148341</v>
       </c>
     </row>
@@ -6021,7 +6021,7 @@
       <c r="AH45" s="5">
         <v>7.1547223484764499</v>
       </c>
-      <c r="AI45">
+      <c r="AI45" s="5">
         <v>389.3833411594232</v>
       </c>
     </row>
@@ -6128,7 +6128,7 @@
       <c r="AH46" s="5">
         <v>6.6944445381975832</v>
       </c>
-      <c r="AI46">
+      <c r="AI46" s="5">
         <v>344.61333842054012</v>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
       <c r="AH47" s="5">
         <v>4.4341667553409936</v>
       </c>
-      <c r="AI47">
+      <c r="AI47" s="5">
         <v>514.92334158072867</v>
       </c>
     </row>
@@ -6342,7 +6342,7 @@
       <c r="AH48" s="5">
         <v>4.5591666952189476</v>
       </c>
-      <c r="AI48">
+      <c r="AI48" s="5">
         <v>422.96667394911248</v>
       </c>
     </row>
@@ -6449,7 +6449,7 @@
       <c r="AH49" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI49">
+      <c r="AI49" s="5">
         <v>702.19001223693294</v>
       </c>
     </row>
@@ -6556,7 +6556,7 @@
       <c r="AH50" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI50">
+      <c r="AI50" s="5">
         <v>669.66001015752556</v>
       </c>
     </row>
@@ -6663,7 +6663,7 @@
       <c r="AH51" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI51">
+      <c r="AI51" s="5">
         <v>669.66001015752556</v>
       </c>
     </row>
@@ -6770,7 +6770,7 @@
       <c r="AH52" s="5">
         <v>11.356389078435798</v>
       </c>
-      <c r="AI52">
+      <c r="AI52" s="5">
         <v>669.66001015752556</v>
       </c>
     </row>
@@ -6877,7 +6877,7 @@
       <c r="AH53" s="5">
         <v>11.009722441848782</v>
       </c>
-      <c r="AI53">
+      <c r="AI53" s="5">
         <v>628.88001114701228</v>
       </c>
     </row>
@@ -6984,7 +6984,7 @@
       <c r="AH54" s="5">
         <v>9.6700001836236975</v>
       </c>
-      <c r="AI54">
+      <c r="AI54" s="5">
         <v>662.87001019318893</v>
       </c>
     </row>
@@ -7091,7 +7091,7 @@
       <c r="AH55" s="5">
         <v>8.4052779038126264</v>
       </c>
-      <c r="AI55">
+      <c r="AI55" s="5">
         <v>702.19001223693294</v>
       </c>
     </row>
@@ -7198,7 +7198,7 @@
       <c r="AH56" s="5">
         <v>7.8900001508080297</v>
       </c>
-      <c r="AI56">
+      <c r="AI56" s="5">
         <v>646.52667742843425</v>
       </c>
     </row>
@@ -7305,7 +7305,7 @@
       <c r="AH57" s="5">
         <v>5.0902778515799181</v>
       </c>
-      <c r="AI57">
+      <c r="AI57" s="5">
         <v>436.14334103912114</v>
       </c>
     </row>
@@ -7412,7 +7412,7 @@
       <c r="AH58" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI58">
+      <c r="AI58" s="5">
         <v>687.9300124709805</v>
       </c>
     </row>
@@ -7519,7 +7519,7 @@
       <c r="AH59" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI59">
+      <c r="AI59" s="5">
         <v>687.9300124709805</v>
       </c>
     </row>
@@ -7626,7 +7626,7 @@
       <c r="AH60" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI60">
+      <c r="AI60" s="5">
         <v>687.9300124709805</v>
       </c>
     </row>
@@ -7733,7 +7733,7 @@
       <c r="AH61" s="5">
         <v>13.238333535359965</v>
       </c>
-      <c r="AI61">
+      <c r="AI61" s="5">
         <v>687.9300124709805</v>
       </c>
     </row>
@@ -7840,7 +7840,7 @@
       <c r="AH62" s="5">
         <v>12.402500250997642</v>
       </c>
-      <c r="AI62">
+      <c r="AI62" s="5">
         <v>656.74667675495152</v>
       </c>
     </row>
@@ -7947,7 +7947,7 @@
       <c r="AH63" s="5">
         <v>13.197500290266342</v>
       </c>
-      <c r="AI63">
+      <c r="AI63" s="5">
         <v>656.12001041024928</v>
       </c>
     </row>
@@ -8054,7 +8054,7 @@
       <c r="AH64" s="5">
         <v>14.578889134505557</v>
       </c>
-      <c r="AI64">
+      <c r="AI64" s="5">
         <v>783.4933441119889</v>
       </c>
     </row>
@@ -8161,7 +8161,7 @@
       <c r="AH65" s="5">
         <v>11.883889088572728</v>
       </c>
-      <c r="AI65">
+      <c r="AI65" s="5">
         <v>683.65334561069801</v>
       </c>
     </row>
@@ -8268,7 +8268,7 @@
       <c r="AH66" s="5">
         <v>12.213611334106988</v>
       </c>
-      <c r="AI66">
+      <c r="AI66" s="5">
         <v>630.5100109905004</v>
       </c>
     </row>
@@ -8375,7 +8375,7 @@
       <c r="AH67" s="5">
         <v>13.395278038394947</v>
       </c>
-      <c r="AI67">
+      <c r="AI67" s="5">
         <v>644.73334439744553</v>
       </c>
     </row>
@@ -8482,7 +8482,7 @@
       <c r="AH68" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI68">
+      <c r="AI68" s="5">
         <v>679.74667786136274</v>
       </c>
     </row>
@@ -8589,7 +8589,7 @@
       <c r="AH69" s="5">
         <v>14.514166940645211</v>
       </c>
-      <c r="AI69">
+      <c r="AI69" s="5">
         <v>715.4333448857069</v>
       </c>
     </row>
@@ -8696,7 +8696,7 @@
       <c r="AH70" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI70">
+      <c r="AI70" s="5">
         <v>679.74667786136274</v>
       </c>
     </row>
@@ -8803,7 +8803,7 @@
       <c r="AH71" s="5">
         <v>14.420555783456399</v>
       </c>
-      <c r="AI71">
+      <c r="AI71" s="5">
         <v>679.74667786136274</v>
       </c>
     </row>
@@ -8910,7 +8910,7 @@
       <c r="AH72" s="5">
         <v>13.200278020401795</v>
       </c>
-      <c r="AI72">
+      <c r="AI72" s="5">
         <v>684.12334228530528</v>
       </c>
     </row>
@@ -9017,7 +9017,7 @@
       <c r="AH73" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI73">
+      <c r="AI73" s="5">
         <v>744.21001186221838</v>
       </c>
     </row>
@@ -9124,7 +9124,7 @@
       <c r="AH74" s="5">
         <v>12.140833531340791</v>
       </c>
-      <c r="AI74">
+      <c r="AI74" s="5">
         <v>744.21001186221838</v>
       </c>
     </row>
@@ -9231,7 +9231,7 @@
       <c r="AH75" s="5">
         <v>12.714166869243813</v>
       </c>
-      <c r="AI75">
+      <c r="AI75" s="5">
         <v>724.0633454682926</v>
       </c>
     </row>
@@ -9338,7 +9338,7 @@
       <c r="AH76" s="5">
         <v>14.380278021987113</v>
       </c>
-      <c r="AI76">
+      <c r="AI76" s="5">
         <v>590.31334434126813</v>
       </c>
     </row>
@@ -9445,7 +9445,7 @@
       <c r="AH77" s="5">
         <v>15.016111336586375</v>
       </c>
-      <c r="AI77">
+      <c r="AI77" s="5">
         <v>628.21667590836682</v>
       </c>
     </row>
@@ -9552,7 +9552,7 @@
       <c r="AH78" s="5">
         <v>14.131666897899574</v>
       </c>
-      <c r="AI78">
+      <c r="AI78" s="5">
         <v>730.94001448949177</v>
       </c>
     </row>
@@ -9659,7 +9659,7 @@
       <c r="AH79" s="5">
         <v>14.880833575605518</v>
       </c>
-      <c r="AI79">
+      <c r="AI79" s="5">
         <v>670.98001096273458</v>
       </c>
     </row>
@@ -9766,7 +9766,7 @@
       <c r="AH80" s="5">
         <v>16.243055798009866</v>
       </c>
-      <c r="AI80">
+      <c r="AI80" s="5">
         <v>1169.4566881649196</v>
       </c>
     </row>
@@ -9873,7 +9873,7 @@
       <c r="AH81" s="5">
         <v>16.389166925619875</v>
       </c>
-      <c r="AI81">
+      <c r="AI81" s="5">
         <v>1255.1900207134584</v>
       </c>
     </row>
@@ -9980,7 +9980,7 @@
       <c r="AH82" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI82">
+      <c r="AI82" s="5">
         <v>1167.3833518219492</v>
       </c>
     </row>
@@ -10087,7 +10087,7 @@
       <c r="AH83" s="5">
         <v>16.020833543212049</v>
       </c>
-      <c r="AI83">
+      <c r="AI83" s="5">
         <v>1167.3833518219492</v>
       </c>
     </row>
@@ -10194,7 +10194,7 @@
       <c r="AH84" s="5">
         <v>15.054166897386313</v>
       </c>
-      <c r="AI84">
+      <c r="AI84" s="5">
         <v>816.7133487234513</v>
       </c>
     </row>
@@ -10301,7 +10301,7 @@
       <c r="AH85" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI85">
+      <c r="AI85" s="5">
         <v>1171.370017160227</v>
       </c>
     </row>
@@ -10408,7 +10408,7 @@
       <c r="AH86" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI86">
+      <c r="AI86" s="5">
         <v>1171.370017160227</v>
       </c>
     </row>
@@ -10515,7 +10515,7 @@
       <c r="AH87" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI87">
+      <c r="AI87" s="5">
         <v>1171.370017160227</v>
       </c>
     </row>
@@ -10622,7 +10622,7 @@
       <c r="AH88" s="5">
         <v>16.396111346284549</v>
       </c>
-      <c r="AI88">
+      <c r="AI88" s="5">
         <v>1227.8800224574904</v>
       </c>
     </row>
@@ -10729,7 +10729,7 @@
       <c r="AH89" s="5">
         <v>15.944722454353339</v>
       </c>
-      <c r="AI89">
+      <c r="AI89" s="5">
         <v>1167.9366861462593</v>
       </c>
     </row>
@@ -10836,7 +10836,7 @@
       <c r="AH90" s="5">
         <v>15.40638912299441</v>
       </c>
-      <c r="AI90">
+      <c r="AI90" s="5">
         <v>1124.8166836957137</v>
       </c>
     </row>
@@ -10943,7 +10943,7 @@
       <c r="AH91" s="5">
         <v>14.980833584670391</v>
       </c>
-      <c r="AI91">
+      <c r="AI91" s="5">
         <v>906.1300134827693</v>
       </c>
     </row>
@@ -11050,7 +11050,7 @@
       <c r="AH92" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI92">
+      <c r="AI92" s="5">
         <v>1100.000017362833</v>
       </c>
     </row>
@@ -11157,7 +11157,7 @@
       <c r="AH93" s="5">
         <v>15.641944691207673</v>
       </c>
-      <c r="AI93">
+      <c r="AI93" s="5">
         <v>1100.000017362833</v>
       </c>
     </row>
@@ -11264,7 +11264,7 @@
       <c r="AH94" s="5">
         <v>15.975278063284026</v>
       </c>
-      <c r="AI94">
+      <c r="AI94" s="5">
         <v>1171.370017160227</v>
       </c>
     </row>
@@ -11371,7 +11371,7 @@
       <c r="AH95" s="5">
         <v>15.691944675313103</v>
       </c>
-      <c r="AI95">
+      <c r="AI95" s="5">
         <v>1101.9933541138967</v>
       </c>
     </row>
@@ -11478,7 +11478,7 @@
       <c r="AH96" s="5">
         <v>15.582500197138224</v>
       </c>
-      <c r="AI96">
+      <c r="AI96" s="5">
         <v>853.43668373152616</v>
       </c>
     </row>
@@ -11585,7 +11585,7 @@
       <c r="AH97" s="5">
         <v>16.058055824786425</v>
       </c>
-      <c r="AI97">
+      <c r="AI97" s="5">
         <v>970.44001293977101</v>
       </c>
     </row>
@@ -11692,7 +11692,7 @@
       <c r="AH98" s="5">
         <v>15.946111321780418</v>
       </c>
-      <c r="AI98">
+      <c r="AI98" s="5">
         <v>996.45668524280188</v>
       </c>
     </row>
@@ -11799,7 +11799,7 @@
       <c r="AH99" s="5">
         <v>16.454722446203231</v>
       </c>
-      <c r="AI99">
+      <c r="AI99" s="5">
         <v>1158.6466879757743</v>
       </c>
     </row>
@@ -11906,7 +11906,7 @@
       <c r="AH100" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI100">
+      <c r="AI100" s="5">
         <v>1412.5500238403679</v>
       </c>
     </row>
@@ -12013,7 +12013,7 @@
       <c r="AH101" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI101">
+      <c r="AI101" s="5">
         <v>1412.5500238403679</v>
       </c>
     </row>
@@ -12120,7 +12120,7 @@
       <c r="AH102" s="5">
         <v>17.015278062555524</v>
       </c>
-      <c r="AI102">
+      <c r="AI102" s="5">
         <v>1412.5500238403679</v>
       </c>
     </row>
@@ -12227,7 +12227,7 @@
       <c r="AH103" s="5">
         <v>15.962500282625358</v>
       </c>
-      <c r="AI103">
+      <c r="AI103" s="5">
         <v>1501.7400254786014</v>
       </c>
     </row>
@@ -12334,7 +12334,7 @@
       <c r="AH104" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI104">
+      <c r="AI104" s="5">
         <v>1429.3566899955272</v>
       </c>
     </row>
@@ -12441,7 +12441,7 @@
       <c r="AH105" s="5">
         <v>17.36972248951594</v>
       </c>
-      <c r="AI105">
+      <c r="AI105" s="5">
         <v>1619.7266931096713</v>
       </c>
     </row>
@@ -12548,7 +12548,7 @@
       <c r="AH106" s="5">
         <v>15.843055815166897</v>
       </c>
-      <c r="AI106">
+      <c r="AI106" s="5">
         <v>1429.3566899955272</v>
       </c>
     </row>
@@ -12655,7 +12655,7 @@
       <c r="AH107" s="5">
         <v>16.991666977935367</v>
       </c>
-      <c r="AI107">
+      <c r="AI107" s="5">
         <v>1461.4566946188609</v>
       </c>
     </row>
@@ -12762,7 +12762,7 @@
       <c r="AH108" s="5">
         <v>17.177500254909198</v>
       </c>
-      <c r="AI108">
+      <c r="AI108" s="5">
         <v>1376.8500243378182</v>
       </c>
     </row>
@@ -12869,7 +12869,7 @@
       <c r="AH109" s="5">
         <v>16.59805584020085</v>
       </c>
-      <c r="AI109">
+      <c r="AI109" s="5">
         <v>1607.316695245107</v>
       </c>
     </row>
@@ -12976,7 +12976,7 @@
       <c r="AH110" s="5">
         <v>18.400555811987982</v>
       </c>
-      <c r="AI110">
+      <c r="AI110" s="5">
         <v>1670.273362938563</v>
       </c>
     </row>
@@ -13083,7 +13083,7 @@
       <c r="AH111" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI111">
+      <c r="AI111" s="5">
         <v>1325.3133495601514</v>
       </c>
     </row>
@@ -13190,7 +13190,7 @@
       <c r="AH112" s="5">
         <v>16.740000236531099</v>
       </c>
-      <c r="AI112">
+      <c r="AI112" s="5">
         <v>1325.3133495601514</v>
       </c>
     </row>
@@ -13297,7 +13297,7 @@
       <c r="AH113" s="5">
         <v>16.237500274015797</v>
       </c>
-      <c r="AI113">
+      <c r="AI113" s="5">
         <v>1339.0533566698432</v>
       </c>
     </row>
@@ -13404,7 +13404,7 @@
       <c r="AH114" s="5">
         <v>16.611111394564311</v>
       </c>
-      <c r="AI114">
+      <c r="AI114" s="5">
         <v>1451.9166888972125</v>
       </c>
     </row>
@@ -13511,7 +13511,7 @@
       <c r="AH115" s="5">
         <v>16.962222494681676</v>
       </c>
-      <c r="AI115">
+      <c r="AI115" s="5">
         <v>1551.293354121844</v>
       </c>
     </row>
@@ -13618,7 +13618,7 @@
       <c r="AH116" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI116">
+      <c r="AI116" s="5">
         <v>1504.2333610216776</v>
       </c>
     </row>
@@ -13725,7 +13725,7 @@
       <c r="AH117" s="5">
         <v>16.695555837617981</v>
       </c>
-      <c r="AI117">
+      <c r="AI117" s="5">
         <v>1504.2333610216776</v>
       </c>
     </row>
@@ -13832,7 +13832,7 @@
       <c r="AH118" s="5">
         <v>17.300555813312531</v>
       </c>
-      <c r="AI118">
+      <c r="AI118" s="5">
         <v>1707.6833669265111</v>
       </c>
     </row>
@@ -13939,7 +13939,7 @@
       <c r="AH119" s="5">
         <v>16.892500269412995</v>
       </c>
-      <c r="AI119">
+      <c r="AI119" s="5">
         <v>1603.7033581415812</v>
       </c>
     </row>
@@ -14046,7 +14046,7 @@
       <c r="AH120" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI120">
+      <c r="AI120" s="5">
         <v>1540.4100324869155</v>
       </c>
     </row>
@@ -14153,7 +14153,7 @@
       <c r="AH121" s="5">
         <v>16.579166912370258</v>
       </c>
-      <c r="AI121">
+      <c r="AI121" s="5">
         <v>1540.4100324869155</v>
       </c>
     </row>
@@ -14260,7 +14260,7 @@
       <c r="AH122" s="5">
         <v>17.377222496933406</v>
       </c>
-      <c r="AI122">
+      <c r="AI122" s="5">
         <v>1612.0533617973329</v>
       </c>
     </row>
@@ -14367,7 +14367,7 @@
       <c r="AH123" s="5">
         <v>18.61972255706787</v>
       </c>
-      <c r="AI123">
+      <c r="AI123" s="5">
         <v>1583.2933620850245</v>
       </c>
     </row>
@@ -14474,7 +14474,7 @@
       <c r="AH124" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI124">
+      <c r="AI124" s="5">
         <v>1782.6833617116015</v>
       </c>
     </row>
@@ -14581,7 +14581,7 @@
       <c r="AH125" s="5">
         <v>21.330278105205959</v>
       </c>
-      <c r="AI125">
+      <c r="AI125" s="5">
         <v>1417.5933627367019</v>
       </c>
     </row>
@@ -14688,7 +14688,7 @@
       <c r="AH126" s="5">
         <v>22.258055904176501</v>
       </c>
-      <c r="AI126">
+      <c r="AI126" s="5">
         <v>1782.6833617116015</v>
       </c>
     </row>
@@ -14795,7 +14795,7 @@
       <c r="AH127" s="5">
         <v>14.705277992950545</v>
       </c>
-      <c r="AI127">
+      <c r="AI127" s="5">
         <v>654.54667957797642</v>
       </c>
     </row>
@@ -14902,7 +14902,7 @@
       <c r="AH128" s="5">
         <v>15.146666885043183</v>
       </c>
-      <c r="AI128">
+      <c r="AI128" s="5">
         <v>613.37334387948113</v>
       </c>
     </row>
@@ -15009,7 +15009,7 @@
       <c r="AH129" s="5">
         <v>15.114166894327436</v>
       </c>
-      <c r="AI129">
+      <c r="AI129" s="5">
         <v>663.24001225084066</v>
       </c>
     </row>
@@ -15116,7 +15116,7 @@
       <c r="AH130" s="5">
         <v>14.685000222010745</v>
       </c>
-      <c r="AI130">
+      <c r="AI130" s="5">
         <v>619.34667505845425</v>
       </c>
     </row>
@@ -15223,7 +15223,7 @@
       <c r="AH131" s="5">
         <v>14.560555819484096</v>
       </c>
-      <c r="AI131">
+      <c r="AI131" s="5">
         <v>583.81001118198037</v>
       </c>
     </row>
@@ -15330,7 +15330,7 @@
       <c r="AH132" s="5">
         <v>14.925000269276401</v>
       </c>
-      <c r="AI132">
+      <c r="AI132" s="5">
         <v>705.52334533234432</v>
       </c>
     </row>
@@ -15437,7 +15437,7 @@
       <c r="AH133" s="5">
         <v>14.240833549056616</v>
       </c>
-      <c r="AI133">
+      <c r="AI133" s="5">
         <v>694.26334502796328</v>
       </c>
     </row>
@@ -15544,7 +15544,7 @@
       <c r="AH134" s="5">
         <v>15.481111367895371</v>
       </c>
-      <c r="AI134">
+      <c r="AI134" s="5">
         <v>796.98001470267775</v>
       </c>
     </row>
@@ -15651,7 +15651,7 @@
       <c r="AH135" s="5">
         <v>15.808611411021815</v>
       </c>
-      <c r="AI135">
+      <c r="AI135" s="5">
         <v>878.90668233633039</v>
       </c>
     </row>
@@ -15758,7 +15758,7 @@
       <c r="AH136" s="5">
         <v>16.348055789868038</v>
       </c>
-      <c r="AI136">
+      <c r="AI136" s="5">
         <v>847.81001371790967</v>
       </c>
     </row>
@@ -15865,7 +15865,7 @@
       <c r="AH137" s="5">
         <v>13.885278014466166</v>
       </c>
-      <c r="AI137">
+      <c r="AI137" s="5">
         <v>578.90334290241196</v>
       </c>
     </row>
@@ -15972,7 +15972,7 @@
       <c r="AH138" s="5">
         <v>17.218055825101004</v>
       </c>
-      <c r="AI138">
+      <c r="AI138" s="5">
         <v>1247.3300210356713</v>
       </c>
     </row>
@@ -16079,7 +16079,7 @@
       <c r="AH139" s="5">
         <v>17.671944708956612</v>
       </c>
-      <c r="AI139">
+      <c r="AI139" s="5">
         <v>1440.4833574632803</v>
       </c>
     </row>
@@ -16186,7 +16186,7 @@
       <c r="AH140" s="5">
         <v>17.840000283055836</v>
       </c>
-      <c r="AI140">
+      <c r="AI140" s="5">
         <v>1479.7433575078844</v>
       </c>
     </row>
@@ -16293,7 +16293,7 @@
       <c r="AH141" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI141">
+      <c r="AI141" s="5">
         <v>2196.9867067073783</v>
       </c>
     </row>
@@ -16400,7 +16400,7 @@
       <c r="AH142" s="5">
         <v>22.653055906295776</v>
       </c>
-      <c r="AI142">
+      <c r="AI142" s="5">
         <v>2196.9867067073783</v>
       </c>
     </row>
@@ -16507,7 +16507,7 @@
       <c r="AH143" s="5">
         <v>22.497500356038412</v>
       </c>
-      <c r="AI143">
+      <c r="AI143" s="5">
         <v>1748.520027906696</v>
       </c>
     </row>
@@ -16614,7 +16614,7 @@
       <c r="AH144" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI144">
+      <c r="AI144" s="5">
         <v>1001.1966831016044</v>
       </c>
     </row>
@@ -16721,7 +16721,7 @@
       <c r="AH145" s="5">
         <v>14.810278096463945</v>
       </c>
-      <c r="AI145">
+      <c r="AI145" s="5">
         <v>1001.1966831016044</v>
       </c>
     </row>
@@ -16828,7 +16828,7 @@
       <c r="AH146" s="5">
         <v>16.466389189826117</v>
       </c>
-      <c r="AI146">
+      <c r="AI146" s="5">
         <v>1009.2633496473233</v>
       </c>
     </row>
@@ -16935,7 +16935,7 @@
       <c r="AH147" s="5">
         <v>18.550555888811747</v>
       </c>
-      <c r="AI147">
+      <c r="AI147" s="5">
         <v>1105.6566875979304</v>
       </c>
     </row>
@@ -17042,7 +17042,7 @@
       <c r="AH148" s="5">
         <v>16.811666933695474</v>
       </c>
-      <c r="AI148">
+      <c r="AI148" s="5">
         <v>927.98334970076883</v>
       </c>
     </row>
@@ -17149,7 +17149,7 @@
       <c r="AH149" s="5">
         <v>16.939166976345909</v>
       </c>
-      <c r="AI149">
+      <c r="AI149" s="5">
         <v>983.30335068504019</v>
       </c>
     </row>
@@ -17256,7 +17256,7 @@
       <c r="AH150" s="5">
         <v>17.050555853048959</v>
       </c>
-      <c r="AI150">
+      <c r="AI150" s="5">
         <v>1071.2700172980626</v>
       </c>
     </row>
@@ -17363,7 +17363,7 @@
       <c r="AH151" s="5">
         <v>18.485833643542396</v>
       </c>
-      <c r="AI151">
+      <c r="AI151" s="5">
         <v>1046.4833499987919</v>
       </c>
     </row>
@@ -17470,7 +17470,7 @@
       <c r="AH152" s="5">
         <v>17.482500301467049</v>
       </c>
-      <c r="AI152">
+      <c r="AI152" s="5">
         <v>1032.8100182595351</v>
       </c>
     </row>
@@ -17577,7 +17577,7 @@
       <c r="AH153" s="5">
         <v>17.544166929192013</v>
       </c>
-      <c r="AI153">
+      <c r="AI153" s="5">
         <v>1064.7866849660873</v>
       </c>
     </row>
@@ -17684,7 +17684,7 @@
       <c r="AH154" s="5">
         <v>17.002222526735729</v>
       </c>
-      <c r="AI154">
+      <c r="AI154" s="5">
         <v>1089.0833561579386</v>
       </c>
     </row>
@@ -17791,7 +17791,7 @@
       <c r="AH155" s="5">
         <v>16.162500272856818</v>
       </c>
-      <c r="AI155">
+      <c r="AI155" s="5">
         <v>1124.6000175555548</v>
       </c>
     </row>
@@ -17898,7 +17898,7 @@
       <c r="AH156" s="5">
         <v>13.510278080569373</v>
       </c>
-      <c r="AI156">
+      <c r="AI156" s="5">
         <v>945.16001687819755</v>
       </c>
     </row>
@@ -18005,7 +18005,7 @@
       <c r="AH157" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI157">
+      <c r="AI157" s="5">
         <v>659.65667902901771</v>
       </c>
     </row>
@@ -18112,7 +18112,7 @@
       <c r="AH158" s="5">
         <v>13.560555803134209</v>
       </c>
-      <c r="AI158">
+      <c r="AI158" s="5">
         <v>659.65667902901771</v>
       </c>
     </row>
@@ -18219,7 +18219,7 @@
       <c r="AH159" s="5">
         <v>11.430000214464963</v>
       </c>
-      <c r="AI159">
+      <c r="AI159" s="5">
         <v>557.09334369699161</v>
       </c>
     </row>
@@ -18326,7 +18326,7 @@
       <c r="AH160" s="5">
         <v>7.7977779119999875</v>
       </c>
-      <c r="AI160">
+      <c r="AI160" s="5">
         <v>365.87333956112462</v>
       </c>
     </row>
@@ -18433,7 +18433,7 @@
       <c r="AH161" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI161">
+      <c r="AI161" s="5">
         <v>223.68333710978428</v>
       </c>
     </row>
@@ -18540,7 +18540,7 @@
       <c r="AH162" s="5">
         <v>7.6125001351452539</v>
       </c>
-      <c r="AI162">
+      <c r="AI162" s="5">
         <v>381.98667274763187</v>
       </c>
     </row>
@@ -18647,7 +18647,7 @@
       <c r="AH163" s="5">
         <v>9.9055557702357575</v>
       </c>
-      <c r="AI163">
+      <c r="AI163" s="5">
         <v>223.68333710978428</v>
       </c>
     </row>
@@ -18754,7 +18754,7 @@
       <c r="AH164" s="5">
         <v>5.8491667841457655</v>
       </c>
-      <c r="AI164">
+      <c r="AI164" s="5">
         <v>220.42333756213387</v>
       </c>
     </row>
@@ -18861,7 +18861,7 @@
       <c r="AH165" s="5">
         <v>4.4586112032747929</v>
       </c>
-      <c r="AI165">
+      <c r="AI165" s="5">
         <v>232.46667109852035</v>
       </c>
     </row>
@@ -18968,7 +18968,7 @@
       <c r="AH166" s="5">
         <v>5.5380556673639347</v>
       </c>
-      <c r="AI166">
+      <c r="AI166" s="5">
         <v>208.14667010505994</v>
       </c>
     </row>

</xml_diff>